<commit_message>
defBoard() Deleted. printDefaultBoard() deleted. Radical rethink and fresh approach. Revisit PIJ Day 5 Arrays, Excercise 4: Creating Matrices
</commit_message>
<xml_diff>
--- a/Ancillary Docs/Default Board Helper File.xlsx
+++ b/Ancillary Docs/Default Board Helper File.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/xeon2035/Desktop/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/xeon2035/Library/Mobile Documents/com~apple~CloudDocs/UniWerk/SkraBBKle/Ancillary Docs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BBD3370D-BAD6-1845-BA0C-4B3EB79D73F1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A2439FAB-DF00-EF4A-BF54-4CFF66EE5C43}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="60" yWindow="500" windowWidth="26740" windowHeight="13940" xr2:uid="{F938695B-E880-FB4D-B508-A292FAB83920}"/>
+    <workbookView xWindow="60" yWindow="500" windowWidth="26740" windowHeight="14620" xr2:uid="{F938695B-E880-FB4D-B508-A292FAB83920}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="273" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="289" uniqueCount="34">
   <si>
     <t>a</t>
   </si>
@@ -107,9 +107,6 @@
     <t>(3)</t>
   </si>
   <si>
-    <t>My little helper file. A visual representation of the default board where s = 16 (16 x 16)</t>
-  </si>
-  <si>
     <t>{0}</t>
   </si>
   <si>
@@ -138,6 +135,9 @@
   </si>
   <si>
     <t>{16}</t>
+  </si>
+  <si>
+    <t>A visual representation of the default board where s = 16 (16 x 16)</t>
   </si>
 </sst>
 </file>
@@ -188,7 +188,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -199,11 +199,14 @@
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -560,21 +563,21 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{86D4BB79-E43C-6E4E-948B-91B0015F6673}">
-  <dimension ref="A1:V17"/>
+  <dimension ref="A1:W18"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="176" zoomScaleNormal="176" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A6" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="Q17" sqref="A1:Q17"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="R18" sqref="A1:R18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="19" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="17" width="3.6640625" style="3" customWidth="1"/>
-    <col min="18" max="18" width="3.5" style="1" customWidth="1"/>
-    <col min="19" max="16384" width="10.83203125" style="1"/>
+    <col min="18" max="19" width="3.5" style="1" customWidth="1"/>
+    <col min="20" max="16384" width="10.83203125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:22" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:23" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="2"/>
       <c r="B1" s="2" t="s">
         <v>0</v>
@@ -624,8 +627,10 @@
       <c r="Q1" s="2" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="2" spans="1:22" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="R1" s="2"/>
+      <c r="S1" s="6"/>
+    </row>
+    <row r="2" spans="1:23" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="2">
         <v>1</v>
       </c>
@@ -677,14 +682,18 @@
       <c r="Q2" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="S2" s="5" t="s">
-        <v>23</v>
-      </c>
-      <c r="T2" s="5"/>
+      <c r="R2" s="2">
+        <v>1</v>
+      </c>
+      <c r="S2" s="6"/>
+      <c r="T2" s="5" t="s">
+        <v>33</v>
+      </c>
       <c r="U2" s="5"/>
       <c r="V2" s="5"/>
-    </row>
-    <row r="3" spans="1:22" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="W2" s="5"/>
+    </row>
+    <row r="3" spans="1:23" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="2">
         <v>2</v>
       </c>
@@ -736,12 +745,16 @@
       <c r="Q3" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="S3" s="5"/>
+      <c r="R3" s="2">
+        <v>2</v>
+      </c>
+      <c r="S3" s="6"/>
       <c r="T3" s="5"/>
       <c r="U3" s="5"/>
       <c r="V3" s="5"/>
-    </row>
-    <row r="4" spans="1:22" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="W3" s="5"/>
+    </row>
+    <row r="4" spans="1:23" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="2">
         <v>3</v>
       </c>
@@ -793,12 +806,16 @@
       <c r="Q4" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="S4" s="5"/>
+      <c r="R4" s="2">
+        <v>3</v>
+      </c>
+      <c r="S4" s="6"/>
       <c r="T4" s="5"/>
       <c r="U4" s="5"/>
       <c r="V4" s="5"/>
-    </row>
-    <row r="5" spans="1:22" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="W4" s="5"/>
+    </row>
+    <row r="5" spans="1:23" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="2">
         <v>4</v>
       </c>
@@ -850,12 +867,16 @@
       <c r="Q5" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="S5" s="5"/>
+      <c r="R5" s="2">
+        <v>4</v>
+      </c>
+      <c r="S5" s="6"/>
       <c r="T5" s="5"/>
       <c r="U5" s="5"/>
       <c r="V5" s="5"/>
-    </row>
-    <row r="6" spans="1:22" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="W5" s="5"/>
+    </row>
+    <row r="6" spans="1:23" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="2">
         <v>5</v>
       </c>
@@ -893,7 +914,7 @@
         <v>16</v>
       </c>
       <c r="M6" s="2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="N6" s="2" t="s">
         <v>16</v>
@@ -907,12 +928,16 @@
       <c r="Q6" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="S6" s="5"/>
+      <c r="R6" s="2">
+        <v>5</v>
+      </c>
+      <c r="S6" s="6"/>
       <c r="T6" s="5"/>
       <c r="U6" s="5"/>
       <c r="V6" s="5"/>
-    </row>
-    <row r="7" spans="1:22" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="W6" s="5"/>
+    </row>
+    <row r="7" spans="1:23" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="2">
         <v>6</v>
       </c>
@@ -964,12 +989,16 @@
       <c r="Q7" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="S7" s="5"/>
+      <c r="R7" s="2">
+        <v>6</v>
+      </c>
+      <c r="S7" s="6"/>
       <c r="T7" s="5"/>
       <c r="U7" s="5"/>
       <c r="V7" s="5"/>
-    </row>
-    <row r="8" spans="1:22" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="W7" s="5"/>
+    </row>
+    <row r="8" spans="1:23" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="2">
         <v>7</v>
       </c>
@@ -1021,8 +1050,12 @@
       <c r="Q8" s="2" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="9" spans="1:22" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="R8" s="2">
+        <v>7</v>
+      </c>
+      <c r="S8" s="6"/>
+    </row>
+    <row r="9" spans="1:23" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="2">
         <v>8</v>
       </c>
@@ -1030,7 +1063,7 @@
         <v>22</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D9" s="2" t="s">
         <v>16</v>
@@ -1063,19 +1096,23 @@
         <v>16</v>
       </c>
       <c r="N9" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="O9" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="P9" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="Q9" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="O9" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="P9" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="Q9" s="2" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="10" spans="1:22" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="R9" s="2">
+        <v>8</v>
+      </c>
+      <c r="S9" s="6"/>
+    </row>
+    <row r="10" spans="1:23" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="2">
         <v>9</v>
       </c>
@@ -1127,8 +1164,12 @@
       <c r="Q10" s="2" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="11" spans="1:22" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="R10" s="2">
+        <v>9</v>
+      </c>
+      <c r="S10" s="6"/>
+    </row>
+    <row r="11" spans="1:23" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="2">
         <v>10</v>
       </c>
@@ -1180,8 +1221,12 @@
       <c r="Q11" s="2" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="12" spans="1:22" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="R11" s="2">
+        <v>10</v>
+      </c>
+      <c r="S11" s="6"/>
+    </row>
+    <row r="12" spans="1:23" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="2">
         <v>11</v>
       </c>
@@ -1233,8 +1278,12 @@
       <c r="Q12" s="2" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="13" spans="1:22" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="R12" s="2">
+        <v>11</v>
+      </c>
+      <c r="S12" s="6"/>
+    </row>
+    <row r="13" spans="1:23" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="2">
         <v>12</v>
       </c>
@@ -1251,32 +1300,32 @@
         <v>16</v>
       </c>
       <c r="F13" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="G13" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="H13" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="I13" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="J13" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="G13" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="H13" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="I13" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="J13" s="2" t="s">
+      <c r="K13" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="L13" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="M13" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="N13" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="K13" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="L13" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="M13" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="N13" s="2" t="s">
-        <v>30</v>
-      </c>
       <c r="O13" s="2" t="s">
         <v>16</v>
       </c>
@@ -1286,8 +1335,12 @@
       <c r="Q13" s="2" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="14" spans="1:22" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="R13" s="2">
+        <v>12</v>
+      </c>
+      <c r="S13" s="6"/>
+    </row>
+    <row r="14" spans="1:23" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="2">
         <v>13</v>
       </c>
@@ -1319,7 +1372,7 @@
         <v>16</v>
       </c>
       <c r="K14" s="2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="L14" s="2" t="s">
         <v>16</v>
@@ -1339,8 +1392,12 @@
       <c r="Q14" s="2" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="15" spans="1:22" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="R14" s="2">
+        <v>13</v>
+      </c>
+      <c r="S14" s="6"/>
+    </row>
+    <row r="15" spans="1:23" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="2">
         <v>14</v>
       </c>
@@ -1392,8 +1449,12 @@
       <c r="Q15" s="2" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="16" spans="1:22" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="R15" s="2">
+        <v>14</v>
+      </c>
+      <c r="S15" s="6"/>
+    </row>
+    <row r="16" spans="1:23" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="2">
         <v>15</v>
       </c>
@@ -1401,7 +1462,7 @@
         <v>16</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D16" s="2" t="s">
         <v>16</v>
@@ -1443,10 +1504,14 @@
         <v>16</v>
       </c>
       <c r="Q16" s="2" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="17" spans="1:17" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+        <v>32</v>
+      </c>
+      <c r="R16" s="2">
+        <v>15</v>
+      </c>
+      <c r="S16" s="6"/>
+    </row>
+    <row r="17" spans="1:19" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" s="2">
         <v>16</v>
       </c>
@@ -1498,24 +1563,81 @@
       <c r="Q17" s="2" t="s">
         <v>16</v>
       </c>
+      <c r="R17" s="2">
+        <v>16</v>
+      </c>
+      <c r="S17" s="6"/>
+    </row>
+    <row r="18" spans="1:19" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A18" s="2"/>
+      <c r="B18" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C18" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="D18" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="E18" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="F18" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="G18" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="H18" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="I18" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="J18" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="K18" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="L18" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="M18" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="N18" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="O18" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="P18" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="Q18" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="R18" s="2"/>
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="S2:V7"/>
+    <mergeCell ref="T2:W7"/>
   </mergeCells>
-  <conditionalFormatting sqref="A1:Q11 I12:Q12 A12:G12 A13:Q1048576">
+  <conditionalFormatting sqref="A1:Q11 A12:G12 I12:Q12 A13:Q17 R1:S17 A19:Q1048576 A18:R18">
     <cfRule type="containsText" dxfId="1" priority="2" operator="containsText" text="{">
       <formula>NOT(ISERROR(SEARCH("{",A1)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B1:Q11 I12:Q12 B12:G12 B13:Q1048576">
+  <conditionalFormatting sqref="B1:Q11 B12:G12 I12:Q12 B13:Q1048576">
     <cfRule type="containsText" dxfId="0" priority="1" operator="containsText" text="(">
       <formula>NOT(ISERROR(SEARCH("(",B1)))</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
   <ignoredErrors>
-    <ignoredError sqref="N2 F2" numberStoredAsText="1"/>
+    <ignoredError sqref="I4" numberStoredAsText="1"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Boardint() Modify: change Check if input element contains {, if so, includes all other elements after it as one elelment toill it gets to } inclusive. Appends } to end of string and writes as one element to 2d Array
</commit_message>
<xml_diff>
--- a/Ancillary Docs/Default Board Helper File.xlsx
+++ b/Ancillary Docs/Default Board Helper File.xlsx
@@ -8,12 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/xeon2035/Library/Mobile Documents/com~apple~CloudDocs/UniWerk/SkraBBKle/Ancillary Docs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A2439FAB-DF00-EF4A-BF54-4CFF66EE5C43}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EAFCEE46-9F7C-8243-82D4-ED629FFEAB1C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="60" yWindow="500" windowWidth="26740" windowHeight="14620" xr2:uid="{F938695B-E880-FB4D-B508-A292FAB83920}"/>
+    <workbookView xWindow="60" yWindow="500" windowWidth="26740" windowHeight="14620" activeTab="1" xr2:uid="{F938695B-E880-FB4D-B508-A292FAB83920}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="BOARD 16" sheetId="1" r:id="rId1"/>
+    <sheet name="BOARD 11" sheetId="3" r:id="rId2"/>
+    <sheet name="Test Data 16x16" sheetId="2" r:id="rId3"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -36,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="289" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="438" uniqueCount="43">
   <si>
     <t>a</t>
   </si>
@@ -138,15 +140,129 @@
   </si>
   <si>
     <t>A visual representation of the default board where s = 16 (16 x 16)</t>
+  </si>
+  <si>
+    <t>16
+.{12}..(2)...{3}...(2)..{8}
+..{2}...(3)...(3)...{2}.
+...{2}...(2).(2)...{2}..
+.(2)..{2}...(2)...{2}..(2)
+.....{2}.....{0}....
+..(3)...(3)...(3)...(3).
+...(2)...(2).(2)...(2)..
+(3){-3}..(2)...{2}...(-4)..{-2}
+...(2)...(2).(2)...(2)..
+..(3)...(3)...(3)...(3).
+.....{2}.....{2}....a
+.(2)..{-1}...(0)...{-1}..(2)
+...{2}...(2).(9)...{2}..
+..{2}...(3)...(3)...{2}.
+.{9}..(2)...{3}...(2)..{16}
+........(3).......</t>
+  </si>
+  <si>
+    <t>16
+…………….
+…………….
+…………….
+…………….
+…………….
+…………….
+…………….
+…………….
+…………….
+…………….
+…………….
+…………….
+…………….
+…………….
+…………….
+…………….</t>
+  </si>
+  <si>
+    <t>16
+BBBBBBBBBBBBBBBB
+BBBBBBBBBBBBBBBB
+BBBBBBBBBBBBBBBB
+BBBBBBBBBBBBBBBB
+BBBBBBBBBBBBBBBB
+BBBBBBBBBBBBBBBB
+BBBBBBBBBBBBBBBB
+BBBBBBBBBBBBBBBB
+BBBBBBBBBBBBBBBB
+BBBBBBBBBBBBBBBB
+BBBBBBBBBBBBBBBB
+BBBBBBBBBBBBBBBB
+BBBBBBBBBBBBBBBB
+BBBBBBBBBBBBBBBB
+BBBBBBBBBBBBBBBB
+BBBBBBBBBBBBBBBB</t>
+  </si>
+  <si>
+    <t>16
+(C)(C)(C)(C)(C)(C)(C)(C)(C)(C)(C)(C)(C)(C)(C)(C)
+(C)(C)(C)(C)(C)(C)(C)(C)(C)(C)(C)(C)(C)(C)(C)(C)
+(C)(C)(C)(C)(C)(C)(C)(C)(C)(C)(C)(C)(C)(C)(C)(C)
+(C)(C)(C)(C)(C)(C)(C)(C)(C)(C)(C)(C)(C)(C)(C)(C)
+(C)(C)(C)(C)(C)(C)(C)(C)(C)(C)(C)(C)(C)(C)(C)(C)
+(C)(C)(C)(C)(C)(C)(C)(C)(C)(C)(C)(C)(C)(C)(C)(C)
+(C)(C)(C)(C)(C)(C)(C)(C)(C)(C)(C)(C)(C)(C)(C)(C)
+(C)(C)(C)(C)(C)(C)(C)(C)(C)(C)(C)(C)(C)(C)(C)(C)
+(C)(C)(C)(C)(C)(C)(C)(C)(C)(C)(C)(C)(C)(C)(C)(C)
+(C)(C)(C)(C)(C)(C)(C)(C)(C)(C)(C)(C)(C)(C)(C)(C)
+(C)(C)(C)(C)(C)(C)(C)(C)(C)(C)(C)(C)(C)(C)(C)(C)
+(C)(C)(C)(C)(C)(C)(C)(C)(C)(C)(C)(C)(C)(C)(C)(C)
+(C)(C)(C)(C)(C)(C)(C)(C)(C)(C)(C)(C)(C)(C)(C)(C)
+(C)(C)(C)(C)(C)(C)(C)(C)(C)(C)(C)(C)(C)(C)(C)(C)
+(C)(C)(C)(C)(C)(C)(C)(C)(C)(C)(C)(C)(C)(C)(C)(C)
+(C)(C)(C)(C)(C)(C)(C)(C)(C)(C)(C)(C)(C)(C)(C)(C)</t>
+  </si>
+  <si>
+    <t>16
+{-4}{-4}{-4}{-4}{-4}{-4}{-4}{-4}{-4}{-4}{-4}{-4}{-4}{-4}{-4}{-4}
+{-4}{-4}{-4}{-4}{-4}{-4}{-4}{-4}{-4}{-4}{-4}{-4}{-4}{-4}{-4}{-4}
+{-4}{-4}{-4}{-4}{-4}{-4}{-4}{-4}{-4}{-4}{-4}{-4}{-4}{-4}{-4}{-4}
+{-4}{-4}{-4}{-4}{-4}{-4}{-4}{-4}{-4}{-4}{-4}{-4}{-4}{-4}{-4}{-4}
+{-4}{-4}{-4}{-4}{-4}{-4}{-4}{-4}{-4}{-4}{-4}{-4}{-4}{-4}{-4}{-4}
+{-4}{-4}{-4}{-4}{-4}{-4}{-4}{-4}{-4}{-4}{-4}{-4}{-4}{-4}{-4}{-4}
+{-4}{-4}{-4}{-4}{-4}{-4}{-4}{-4}{-4}{-4}{-4}{-4}{-4}{-4}{-4}{-4}
+{-4}{-4}{-4}{-4}{-4}{-4}{-4}{-4}{-4}{-4}{-4}{-4}{-4}{-4}{-4}{-4}
+{-4}{-4}{-4}{-4}{-4}{-4}{-4}{-4}{-4}{-4}{-4}{-4}{-4}{-4}{-4}{-4}
+{-4}{-4}{-4}{-4}{-4}{-4}{-4}{-4}{-4}{-4}{-4}{-4}{-4}{-4}{-4}{-4}
+{-4}{-4}{-4}{-4}{-4}{-4}{-4}{-4}{-4}{-4}{-4}{-4}{-4}{-4}{-4}{-4}
+{-4}{-4}{-4}{-4}{-4}{-4}{-4}{-4}{-4}{-4}{-4}{-4}{-4}{-4}{-4}{-4}
+{-4}{-4}{-4}{-4}{-4}{-4}{-4}{-4}{-4}{-4}{-4}{-4}{-4}{-4}{-4}{-4}
+{-4}{-4}{-4}{-4}{-4}{-4}{-4}{-4}{-4}{-4}{-4}{-4}{-4}{-4}{-4}{-4}
+{-4}{-4}{-4}{-4}{-4}{-4}{-4}{-4}{-4}{-4}{-4}{-4}{-4}{-4}{-4}{-4}
+{-4}{-4}{-4}{-4}{-4}{-4}{-4}{-4}{-4}{-4}{-4}{-4}{-4}{-4}{-4}{-4}</t>
+  </si>
+  <si>
+    <t>A</t>
+  </si>
+  <si>
+    <t>A visual representation of the default board where s = 11 (11 x 11)</t>
+  </si>
+  <si>
+    <t>{V}</t>
+  </si>
+  <si>
+    <t>{Q}</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
+      <color theme="1"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="15"/>
       <color theme="1"/>
       <name val="Aptos Narrow"/>
       <family val="2"/>
@@ -188,7 +304,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -203,16 +319,45 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="2">
+  <dxfs count="4">
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <color rgb="FF006100"/>
@@ -565,9 +710,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{86D4BB79-E43C-6E4E-948B-91B0015F6673}">
   <dimension ref="A1:W18"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+    <sheetView showGridLines="0" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="R18" sqref="A1:R18"/>
+      <selection pane="bottomLeft" activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="19" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -628,7 +773,7 @@
         <v>15</v>
       </c>
       <c r="R1" s="2"/>
-      <c r="S1" s="6"/>
+      <c r="S1" s="3"/>
     </row>
     <row r="2" spans="1:23" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="2">
@@ -685,13 +830,13 @@
       <c r="R2" s="2">
         <v>1</v>
       </c>
-      <c r="S2" s="6"/>
-      <c r="T2" s="5" t="s">
+      <c r="S2" s="3"/>
+      <c r="T2" s="9" t="s">
         <v>33</v>
       </c>
-      <c r="U2" s="5"/>
-      <c r="V2" s="5"/>
-      <c r="W2" s="5"/>
+      <c r="U2" s="9"/>
+      <c r="V2" s="9"/>
+      <c r="W2" s="9"/>
     </row>
     <row r="3" spans="1:23" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="2">
@@ -748,11 +893,11 @@
       <c r="R3" s="2">
         <v>2</v>
       </c>
-      <c r="S3" s="6"/>
-      <c r="T3" s="5"/>
-      <c r="U3" s="5"/>
-      <c r="V3" s="5"/>
-      <c r="W3" s="5"/>
+      <c r="S3" s="3"/>
+      <c r="T3" s="9"/>
+      <c r="U3" s="9"/>
+      <c r="V3" s="9"/>
+      <c r="W3" s="9"/>
     </row>
     <row r="4" spans="1:23" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="2">
@@ -809,11 +954,11 @@
       <c r="R4" s="2">
         <v>3</v>
       </c>
-      <c r="S4" s="6"/>
-      <c r="T4" s="5"/>
-      <c r="U4" s="5"/>
-      <c r="V4" s="5"/>
-      <c r="W4" s="5"/>
+      <c r="S4" s="3"/>
+      <c r="T4" s="9"/>
+      <c r="U4" s="9"/>
+      <c r="V4" s="9"/>
+      <c r="W4" s="9"/>
     </row>
     <row r="5" spans="1:23" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="2">
@@ -870,11 +1015,11 @@
       <c r="R5" s="2">
         <v>4</v>
       </c>
-      <c r="S5" s="6"/>
-      <c r="T5" s="5"/>
-      <c r="U5" s="5"/>
-      <c r="V5" s="5"/>
-      <c r="W5" s="5"/>
+      <c r="S5" s="3"/>
+      <c r="T5" s="9"/>
+      <c r="U5" s="9"/>
+      <c r="V5" s="9"/>
+      <c r="W5" s="9"/>
     </row>
     <row r="6" spans="1:23" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="2">
@@ -931,11 +1076,11 @@
       <c r="R6" s="2">
         <v>5</v>
       </c>
-      <c r="S6" s="6"/>
-      <c r="T6" s="5"/>
-      <c r="U6" s="5"/>
-      <c r="V6" s="5"/>
-      <c r="W6" s="5"/>
+      <c r="S6" s="3"/>
+      <c r="T6" s="9"/>
+      <c r="U6" s="9"/>
+      <c r="V6" s="9"/>
+      <c r="W6" s="9"/>
     </row>
     <row r="7" spans="1:23" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="2">
@@ -992,11 +1137,11 @@
       <c r="R7" s="2">
         <v>6</v>
       </c>
-      <c r="S7" s="6"/>
-      <c r="T7" s="5"/>
-      <c r="U7" s="5"/>
-      <c r="V7" s="5"/>
-      <c r="W7" s="5"/>
+      <c r="S7" s="3"/>
+      <c r="T7" s="9"/>
+      <c r="U7" s="9"/>
+      <c r="V7" s="9"/>
+      <c r="W7" s="9"/>
     </row>
     <row r="8" spans="1:23" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="2">
@@ -1053,7 +1198,8 @@
       <c r="R8" s="2">
         <v>7</v>
       </c>
-      <c r="S8" s="6"/>
+      <c r="S8" s="3"/>
+      <c r="T8" s="5"/>
     </row>
     <row r="9" spans="1:23" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="2">
@@ -1110,7 +1256,7 @@
       <c r="R9" s="2">
         <v>8</v>
       </c>
-      <c r="S9" s="6"/>
+      <c r="S9" s="3"/>
     </row>
     <row r="10" spans="1:23" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="2">
@@ -1167,7 +1313,7 @@
       <c r="R10" s="2">
         <v>9</v>
       </c>
-      <c r="S10" s="6"/>
+      <c r="S10" s="3"/>
     </row>
     <row r="11" spans="1:23" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="2">
@@ -1224,7 +1370,7 @@
       <c r="R11" s="2">
         <v>10</v>
       </c>
-      <c r="S11" s="6"/>
+      <c r="S11" s="3"/>
     </row>
     <row r="12" spans="1:23" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="2">
@@ -1281,7 +1427,7 @@
       <c r="R12" s="2">
         <v>11</v>
       </c>
-      <c r="S12" s="6"/>
+      <c r="S12" s="3"/>
     </row>
     <row r="13" spans="1:23" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="2">
@@ -1338,7 +1484,7 @@
       <c r="R13" s="2">
         <v>12</v>
       </c>
-      <c r="S13" s="6"/>
+      <c r="S13" s="3"/>
     </row>
     <row r="14" spans="1:23" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="2">
@@ -1395,7 +1541,7 @@
       <c r="R14" s="2">
         <v>13</v>
       </c>
-      <c r="S14" s="6"/>
+      <c r="S14" s="3"/>
     </row>
     <row r="15" spans="1:23" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="2">
@@ -1452,7 +1598,7 @@
       <c r="R15" s="2">
         <v>14</v>
       </c>
-      <c r="S15" s="6"/>
+      <c r="S15" s="3"/>
     </row>
     <row r="16" spans="1:23" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="2">
@@ -1509,7 +1655,7 @@
       <c r="R16" s="2">
         <v>15</v>
       </c>
-      <c r="S16" s="6"/>
+      <c r="S16" s="3"/>
     </row>
     <row r="17" spans="1:19" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" s="2">
@@ -1566,7 +1712,7 @@
       <c r="R17" s="2">
         <v>16</v>
       </c>
-      <c r="S17" s="6"/>
+      <c r="S17" s="3"/>
     </row>
     <row r="18" spans="1:19" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" s="2"/>
@@ -1624,13 +1770,13 @@
   <mergeCells count="1">
     <mergeCell ref="T2:W7"/>
   </mergeCells>
-  <conditionalFormatting sqref="A1:Q11 A12:G12 I12:Q12 A13:Q17 R1:S17 A19:Q1048576 A18:R18">
-    <cfRule type="containsText" dxfId="1" priority="2" operator="containsText" text="{">
+  <conditionalFormatting sqref="A1:Q11 A12:G12 I12:Q12 A13:Q17 A18:R18 A19:Q1048576 R1:S17">
+    <cfRule type="containsText" dxfId="3" priority="2" operator="containsText" text="{">
       <formula>NOT(ISERROR(SEARCH("{",A1)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B1:Q11 B12:G12 I12:Q12 B13:Q1048576">
-    <cfRule type="containsText" dxfId="0" priority="1" operator="containsText" text="(">
+    <cfRule type="containsText" dxfId="2" priority="1" operator="containsText" text="(">
       <formula>NOT(ISERROR(SEARCH("(",B1)))</formula>
     </cfRule>
   </conditionalFormatting>
@@ -1640,4 +1786,645 @@
     <ignoredError sqref="I4" numberStoredAsText="1"/>
   </ignoredErrors>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6BAE5677-87B1-5C4F-AA9E-8B56D72F0A3D}">
+  <dimension ref="A1:R13"/>
+  <sheetViews>
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A3" sqref="A3:L12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="19" customHeight="1" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="12" width="3.6640625" style="3" customWidth="1"/>
+    <col min="13" max="14" width="3.5" style="1" customWidth="1"/>
+    <col min="15" max="16384" width="10.83203125" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:18" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A1" s="2"/>
+      <c r="B1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="H1" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="I1" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="J1" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="K1" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="L1" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="M1" s="2"/>
+      <c r="N1" s="3"/>
+    </row>
+    <row r="2" spans="1:18" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="2">
+        <v>1</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="F2" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="G2" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="H2" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="I2" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="J2" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="K2" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="L2" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="M2" s="2">
+        <v>1</v>
+      </c>
+      <c r="N2" s="3"/>
+      <c r="O2" s="9" t="s">
+        <v>40</v>
+      </c>
+      <c r="P2" s="9"/>
+      <c r="Q2" s="9"/>
+      <c r="R2" s="9"/>
+    </row>
+    <row r="3" spans="1:18" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A3" s="2">
+        <v>1</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="F3" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="G3" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="H3" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="I3" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="J3" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="K3" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="L3" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="M3" s="2">
+        <v>2</v>
+      </c>
+      <c r="N3" s="3"/>
+      <c r="O3" s="9"/>
+      <c r="P3" s="9"/>
+      <c r="Q3" s="9"/>
+      <c r="R3" s="9"/>
+    </row>
+    <row r="4" spans="1:18" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A4" s="2">
+        <v>1</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="E4" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="F4" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="G4" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="H4" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="I4" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="J4" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="K4" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="L4" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="M4" s="2">
+        <v>3</v>
+      </c>
+      <c r="N4" s="3"/>
+      <c r="O4" s="9"/>
+      <c r="P4" s="9"/>
+      <c r="Q4" s="9"/>
+      <c r="R4" s="9"/>
+    </row>
+    <row r="5" spans="1:18" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A5" s="2">
+        <v>1</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="E5" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="F5" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="G5" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="H5" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="I5" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="J5" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="K5" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="L5" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="M5" s="2">
+        <v>4</v>
+      </c>
+      <c r="N5" s="3"/>
+      <c r="O5" s="9"/>
+      <c r="P5" s="9"/>
+      <c r="Q5" s="9"/>
+      <c r="R5" s="9"/>
+    </row>
+    <row r="6" spans="1:18" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A6" s="2">
+        <v>1</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="E6" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="F6" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="G6" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="H6" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="I6" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="J6" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="K6" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="L6" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="M6" s="2">
+        <v>5</v>
+      </c>
+      <c r="N6" s="3"/>
+      <c r="O6" s="9"/>
+      <c r="P6" s="9"/>
+      <c r="Q6" s="9"/>
+      <c r="R6" s="9"/>
+    </row>
+    <row r="7" spans="1:18" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A7" s="2">
+        <v>1</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="E7" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="F7" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="G7" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="H7" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="I7" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="J7" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="K7" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="L7" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="M7" s="2">
+        <v>6</v>
+      </c>
+      <c r="N7" s="3"/>
+      <c r="O7" s="9"/>
+      <c r="P7" s="9"/>
+      <c r="Q7" s="9"/>
+      <c r="R7" s="9"/>
+    </row>
+    <row r="8" spans="1:18" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A8" s="2">
+        <v>1</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="D8" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="E8" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="F8" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="G8" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="H8" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="I8" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="J8" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="K8" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="L8" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="M8" s="2">
+        <v>7</v>
+      </c>
+      <c r="N8" s="3"/>
+      <c r="O8" s="5"/>
+    </row>
+    <row r="9" spans="1:18" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A9" s="2">
+        <v>1</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="D9" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="E9" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="F9" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="G9" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="H9" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="I9" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="J9" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="K9" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="L9" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="M9" s="2">
+        <v>8</v>
+      </c>
+      <c r="N9" s="3"/>
+    </row>
+    <row r="10" spans="1:18" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A10" s="2">
+        <v>1</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="D10" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="E10" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="F10" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="G10" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="H10" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="I10" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="J10" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="K10" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="L10" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="M10" s="2">
+        <v>9</v>
+      </c>
+      <c r="N10" s="3"/>
+    </row>
+    <row r="11" spans="1:18" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A11" s="2">
+        <v>1</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="C11" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="D11" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="E11" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="F11" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="G11" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="H11" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="I11" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="J11" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="K11" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="L11" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="M11" s="2">
+        <v>10</v>
+      </c>
+      <c r="N11" s="3"/>
+    </row>
+    <row r="12" spans="1:18" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A12" s="2">
+        <v>1</v>
+      </c>
+      <c r="B12" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="C12" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="D12" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="E12" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="F12" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="G12" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="H12" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="I12" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="J12" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="K12" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="L12" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="M12" s="2">
+        <v>11</v>
+      </c>
+      <c r="N12" s="3"/>
+    </row>
+    <row r="13" spans="1:18" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A13" s="2"/>
+      <c r="B13" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C13" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="D13" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="E13" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="F13" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="G13" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="H13" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="I13" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="J13" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="K13" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="L13" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="M13" s="2"/>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="O2:R7"/>
+  </mergeCells>
+  <conditionalFormatting sqref="A14:L1048576 A13:M13 A1:N12">
+    <cfRule type="containsText" dxfId="1" priority="2" operator="containsText" text="{">
+      <formula>NOT(ISERROR(SEARCH("{",A1)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B1:L1048576">
+    <cfRule type="containsText" dxfId="0" priority="1" operator="containsText" text="(">
+      <formula>NOT(ISERROR(SEARCH("(",B1)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{613A7648-F18E-AE44-AC03-528A68E0F000}">
+  <dimension ref="A1:F1"/>
+  <sheetViews>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B1" sqref="B1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="31.33203125" style="6" customWidth="1"/>
+    <col min="2" max="2" width="17.83203125" style="6" customWidth="1"/>
+    <col min="3" max="3" width="22.83203125" style="6" customWidth="1"/>
+    <col min="4" max="4" width="53.1640625" style="6" customWidth="1"/>
+    <col min="5" max="5" width="59.1640625" style="6" customWidth="1"/>
+    <col min="6" max="16384" width="10.83203125" style="6"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" ht="357" x14ac:dyDescent="0.2">
+      <c r="A1" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="B1" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="C1" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="D1" s="7" t="s">
+        <v>37</v>
+      </c>
+      <c r="E1" s="7" t="s">
+        <v>38</v>
+      </c>
+      <c r="F1" s="8"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
boardCustomOrDefault() Change custom filename confirmation
</commit_message>
<xml_diff>
--- a/Ancillary Docs/Default Board Helper File.xlsx
+++ b/Ancillary Docs/Default Board Helper File.xlsx
@@ -5,17 +5,17 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/xeon2035/Library/Mobile Documents/com~apple~CloudDocs/UniWerk/SkraBBKle/Ancillary Docs/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/xeon2035/Library/Mobile Documents/com~apple~CloudDocs/UniWerk/SKraBBKle/Ancillary Docs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EAFCEE46-9F7C-8243-82D4-ED629FFEAB1C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E0DCCCED-1ABE-BF4B-82D6-E040D982814F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="60" yWindow="500" windowWidth="26740" windowHeight="14620" activeTab="1" xr2:uid="{F938695B-E880-FB4D-B508-A292FAB83920}"/>
   </bookViews>
   <sheets>
     <sheet name="BOARD 16" sheetId="1" r:id="rId1"/>
     <sheet name="BOARD 11" sheetId="3" r:id="rId2"/>
-    <sheet name="Test Data 16x16" sheetId="2" r:id="rId3"/>
+    <sheet name="Test Data" sheetId="2" r:id="rId3"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="438" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="439" uniqueCount="42">
   <si>
     <t>a</t>
   </si>
@@ -237,23 +237,42 @@
 {-4}{-4}{-4}{-4}{-4}{-4}{-4}{-4}{-4}{-4}{-4}{-4}{-4}{-4}{-4}{-4}</t>
   </si>
   <si>
-    <t>A</t>
-  </si>
-  <si>
     <t>A visual representation of the default board where s = 11 (11 x 11)</t>
   </si>
   <si>
-    <t>{V}</t>
-  </si>
-  <si>
-    <t>{Q}</t>
+    <t>11
+.{12}..-2...{3}..
+..{2}...(3)...(3)
+...{2}...(2).(2).
+.(2)..{2}...(2)..
+.....{2}.....
+..(3)...(3)...(3)
+...(2)...(2).(2).
+(3){-3)..(2)...{2}..
+...(2)...(2).(2).
+..(3)...(3)...(3)
+.....{2}.....</t>
+  </si>
+  <si>
+    <t>11
+...{3}...(2)..{8}
+.(3)...(3)...{2}.
+..(2).(2)...{2}..
+...(2)...{2}..(2)
+{2}.....{0}....
+.(3)...(3)...(3).
+..(2).(2)...(2)..
+...{2}...(-4)..{-2}
+..(2).(2)...(2)..
+.(3)...(3)...(3).
+{2}.....{2}....</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -268,16 +287,49 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF006100"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF9C0006"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor rgb="FF000000"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor rgb="FF000000"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="2">
+  <borders count="5">
     <border>
       <left/>
       <right/>
@@ -300,11 +352,48 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -333,11 +422,55 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="49" fontId="4" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="4">
+  <dxfs count="6">
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <color rgb="FF006100"/>
@@ -712,7 +845,7 @@
   <sheetViews>
     <sheetView showGridLines="0" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B2" sqref="B2"/>
+      <selection pane="bottomLeft" activeCell="G2" sqref="G2:Q12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="19" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1771,12 +1904,12 @@
     <mergeCell ref="T2:W7"/>
   </mergeCells>
   <conditionalFormatting sqref="A1:Q11 A12:G12 I12:Q12 A13:Q17 A18:R18 A19:Q1048576 R1:S17">
-    <cfRule type="containsText" dxfId="3" priority="2" operator="containsText" text="{">
+    <cfRule type="containsText" dxfId="5" priority="2" operator="containsText" text="{">
       <formula>NOT(ISERROR(SEARCH("{",A1)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B1:Q11 B12:G12 I12:Q12 B13:Q1048576">
-    <cfRule type="containsText" dxfId="2" priority="1" operator="containsText" text="(">
+    <cfRule type="containsText" dxfId="4" priority="1" operator="containsText" text="(">
       <formula>NOT(ISERROR(SEARCH("(",B1)))</formula>
     </cfRule>
   </conditionalFormatting>
@@ -1794,7 +1927,7 @@
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A3" sqref="A3:L12"/>
+      <selection pane="bottomLeft" activeCell="B2" sqref="B2:L12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="19" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1846,45 +1979,45 @@
       <c r="A2" s="2">
         <v>1</v>
       </c>
-      <c r="B2" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="D2" s="2" t="s">
-        <v>41</v>
-      </c>
-      <c r="E2" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="F2" s="4" t="s">
-        <v>39</v>
-      </c>
-      <c r="G2" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="H2" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="I2" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="J2" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="K2" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="L2" s="2" t="s">
-        <v>39</v>
+      <c r="B2" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="C2" s="11" t="s">
+        <v>17</v>
+      </c>
+      <c r="D2" s="12" t="s">
+        <v>16</v>
+      </c>
+      <c r="E2" s="12" t="s">
+        <v>16</v>
+      </c>
+      <c r="F2" s="13">
+        <v>-2</v>
+      </c>
+      <c r="G2" s="12" t="s">
+        <v>16</v>
+      </c>
+      <c r="H2" s="12" t="s">
+        <v>16</v>
+      </c>
+      <c r="I2" s="12" t="s">
+        <v>16</v>
+      </c>
+      <c r="J2" s="11" t="s">
+        <v>18</v>
+      </c>
+      <c r="K2" s="12" t="s">
+        <v>16</v>
+      </c>
+      <c r="L2" s="12" t="s">
+        <v>16</v>
       </c>
       <c r="M2" s="2">
         <v>1</v>
       </c>
       <c r="N2" s="3"/>
       <c r="O2" s="9" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="P2" s="9"/>
       <c r="Q2" s="9"/>
@@ -1894,38 +2027,38 @@
       <c r="A3" s="2">
         <v>1</v>
       </c>
-      <c r="B3" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="C3" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="D3" s="2" t="s">
-        <v>41</v>
-      </c>
-      <c r="E3" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="F3" s="4" t="s">
-        <v>39</v>
-      </c>
-      <c r="G3" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="H3" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="I3" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="J3" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="K3" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="L3" s="2" t="s">
-        <v>39</v>
+      <c r="B3" s="14" t="s">
+        <v>16</v>
+      </c>
+      <c r="C3" s="15" t="s">
+        <v>16</v>
+      </c>
+      <c r="D3" s="11" t="s">
+        <v>21</v>
+      </c>
+      <c r="E3" s="15" t="s">
+        <v>16</v>
+      </c>
+      <c r="F3" s="15" t="s">
+        <v>16</v>
+      </c>
+      <c r="G3" s="15" t="s">
+        <v>16</v>
+      </c>
+      <c r="H3" s="16" t="s">
+        <v>22</v>
+      </c>
+      <c r="I3" s="15" t="s">
+        <v>16</v>
+      </c>
+      <c r="J3" s="15" t="s">
+        <v>16</v>
+      </c>
+      <c r="K3" s="15" t="s">
+        <v>16</v>
+      </c>
+      <c r="L3" s="16" t="s">
+        <v>22</v>
       </c>
       <c r="M3" s="2">
         <v>2</v>
@@ -1940,38 +2073,38 @@
       <c r="A4" s="2">
         <v>1</v>
       </c>
-      <c r="B4" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="C4" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="D4" s="2" t="s">
-        <v>41</v>
-      </c>
-      <c r="E4" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="F4" s="4" t="s">
-        <v>39</v>
-      </c>
-      <c r="G4" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="H4" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="I4" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="J4" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="K4" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="L4" s="2" t="s">
-        <v>39</v>
+      <c r="B4" s="14" t="s">
+        <v>16</v>
+      </c>
+      <c r="C4" s="15" t="s">
+        <v>16</v>
+      </c>
+      <c r="D4" s="15" t="s">
+        <v>16</v>
+      </c>
+      <c r="E4" s="11" t="s">
+        <v>21</v>
+      </c>
+      <c r="F4" s="15" t="s">
+        <v>16</v>
+      </c>
+      <c r="G4" s="15" t="s">
+        <v>16</v>
+      </c>
+      <c r="H4" s="15" t="s">
+        <v>16</v>
+      </c>
+      <c r="I4" s="16" t="s">
+        <v>20</v>
+      </c>
+      <c r="J4" s="15" t="s">
+        <v>16</v>
+      </c>
+      <c r="K4" s="16" t="s">
+        <v>20</v>
+      </c>
+      <c r="L4" s="15" t="s">
+        <v>16</v>
       </c>
       <c r="M4" s="2">
         <v>3</v>
@@ -1986,38 +2119,38 @@
       <c r="A5" s="2">
         <v>1</v>
       </c>
-      <c r="B5" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="C5" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="D5" s="2" t="s">
-        <v>41</v>
-      </c>
-      <c r="E5" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="F5" s="4" t="s">
-        <v>39</v>
-      </c>
-      <c r="G5" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="H5" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="I5" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="J5" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="K5" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="L5" s="2" t="s">
-        <v>39</v>
+      <c r="B5" s="14" t="s">
+        <v>16</v>
+      </c>
+      <c r="C5" s="16" t="s">
+        <v>20</v>
+      </c>
+      <c r="D5" s="15" t="s">
+        <v>16</v>
+      </c>
+      <c r="E5" s="15" t="s">
+        <v>16</v>
+      </c>
+      <c r="F5" s="11" t="s">
+        <v>21</v>
+      </c>
+      <c r="G5" s="15" t="s">
+        <v>16</v>
+      </c>
+      <c r="H5" s="15" t="s">
+        <v>16</v>
+      </c>
+      <c r="I5" s="15" t="s">
+        <v>16</v>
+      </c>
+      <c r="J5" s="16" t="s">
+        <v>20</v>
+      </c>
+      <c r="K5" s="15" t="s">
+        <v>16</v>
+      </c>
+      <c r="L5" s="15" t="s">
+        <v>16</v>
       </c>
       <c r="M5" s="2">
         <v>4</v>
@@ -2032,38 +2165,38 @@
       <c r="A6" s="2">
         <v>1</v>
       </c>
-      <c r="B6" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="C6" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="D6" s="2" t="s">
-        <v>41</v>
-      </c>
-      <c r="E6" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="F6" s="4" t="s">
-        <v>39</v>
-      </c>
-      <c r="G6" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="H6" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="I6" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="J6" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="K6" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="L6" s="2" t="s">
-        <v>39</v>
+      <c r="B6" s="14" t="s">
+        <v>16</v>
+      </c>
+      <c r="C6" s="15" t="s">
+        <v>16</v>
+      </c>
+      <c r="D6" s="15" t="s">
+        <v>16</v>
+      </c>
+      <c r="E6" s="15" t="s">
+        <v>16</v>
+      </c>
+      <c r="F6" s="15" t="s">
+        <v>16</v>
+      </c>
+      <c r="G6" s="11" t="s">
+        <v>21</v>
+      </c>
+      <c r="H6" s="15" t="s">
+        <v>16</v>
+      </c>
+      <c r="I6" s="15" t="s">
+        <v>16</v>
+      </c>
+      <c r="J6" s="15" t="s">
+        <v>16</v>
+      </c>
+      <c r="K6" s="15" t="s">
+        <v>16</v>
+      </c>
+      <c r="L6" s="15" t="s">
+        <v>16</v>
       </c>
       <c r="M6" s="2">
         <v>5</v>
@@ -2078,38 +2211,38 @@
       <c r="A7" s="2">
         <v>1</v>
       </c>
-      <c r="B7" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="C7" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="D7" s="2" t="s">
-        <v>41</v>
-      </c>
-      <c r="E7" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="F7" s="4" t="s">
-        <v>39</v>
-      </c>
-      <c r="G7" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="H7" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="I7" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="J7" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="K7" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="L7" s="2" t="s">
-        <v>39</v>
+      <c r="B7" s="14" t="s">
+        <v>16</v>
+      </c>
+      <c r="C7" s="15" t="s">
+        <v>16</v>
+      </c>
+      <c r="D7" s="16" t="s">
+        <v>22</v>
+      </c>
+      <c r="E7" s="15" t="s">
+        <v>16</v>
+      </c>
+      <c r="F7" s="15" t="s">
+        <v>16</v>
+      </c>
+      <c r="G7" s="15" t="s">
+        <v>16</v>
+      </c>
+      <c r="H7" s="16" t="s">
+        <v>22</v>
+      </c>
+      <c r="I7" s="15" t="s">
+        <v>16</v>
+      </c>
+      <c r="J7" s="15" t="s">
+        <v>16</v>
+      </c>
+      <c r="K7" s="15" t="s">
+        <v>16</v>
+      </c>
+      <c r="L7" s="16" t="s">
+        <v>22</v>
       </c>
       <c r="M7" s="2">
         <v>6</v>
@@ -2124,38 +2257,38 @@
       <c r="A8" s="2">
         <v>1</v>
       </c>
-      <c r="B8" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="C8" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="D8" s="2" t="s">
-        <v>41</v>
-      </c>
-      <c r="E8" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="F8" s="4" t="s">
-        <v>39</v>
-      </c>
-      <c r="G8" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="H8" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="I8" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="J8" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="K8" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="L8" s="2" t="s">
-        <v>39</v>
+      <c r="B8" s="14" t="s">
+        <v>16</v>
+      </c>
+      <c r="C8" s="15" t="s">
+        <v>16</v>
+      </c>
+      <c r="D8" s="15" t="s">
+        <v>16</v>
+      </c>
+      <c r="E8" s="16" t="s">
+        <v>20</v>
+      </c>
+      <c r="F8" s="15" t="s">
+        <v>16</v>
+      </c>
+      <c r="G8" s="15" t="s">
+        <v>16</v>
+      </c>
+      <c r="H8" s="15" t="s">
+        <v>16</v>
+      </c>
+      <c r="I8" s="16" t="s">
+        <v>20</v>
+      </c>
+      <c r="J8" s="15" t="s">
+        <v>16</v>
+      </c>
+      <c r="K8" s="16" t="s">
+        <v>20</v>
+      </c>
+      <c r="L8" s="15" t="s">
+        <v>16</v>
       </c>
       <c r="M8" s="2">
         <v>7</v>
@@ -2167,38 +2300,38 @@
       <c r="A9" s="2">
         <v>1</v>
       </c>
-      <c r="B9" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="C9" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="D9" s="2" t="s">
-        <v>41</v>
-      </c>
-      <c r="E9" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="F9" s="4" t="s">
-        <v>39</v>
-      </c>
-      <c r="G9" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="H9" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="I9" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="J9" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="K9" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="L9" s="2" t="s">
-        <v>39</v>
+      <c r="B9" s="16" t="s">
+        <v>22</v>
+      </c>
+      <c r="C9" s="11" t="s">
+        <v>24</v>
+      </c>
+      <c r="D9" s="15" t="s">
+        <v>16</v>
+      </c>
+      <c r="E9" s="15" t="s">
+        <v>16</v>
+      </c>
+      <c r="F9" s="16" t="s">
+        <v>20</v>
+      </c>
+      <c r="G9" s="15" t="s">
+        <v>16</v>
+      </c>
+      <c r="H9" s="15" t="s">
+        <v>16</v>
+      </c>
+      <c r="I9" s="15" t="s">
+        <v>16</v>
+      </c>
+      <c r="J9" s="11" t="s">
+        <v>21</v>
+      </c>
+      <c r="K9" s="15" t="s">
+        <v>16</v>
+      </c>
+      <c r="L9" s="15" t="s">
+        <v>16</v>
       </c>
       <c r="M9" s="2">
         <v>8</v>
@@ -2209,38 +2342,38 @@
       <c r="A10" s="2">
         <v>1</v>
       </c>
-      <c r="B10" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="C10" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="D10" s="2" t="s">
-        <v>41</v>
-      </c>
-      <c r="E10" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="F10" s="4" t="s">
-        <v>39</v>
-      </c>
-      <c r="G10" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="H10" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="I10" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="J10" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="K10" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="L10" s="2" t="s">
-        <v>39</v>
+      <c r="B10" s="14" t="s">
+        <v>16</v>
+      </c>
+      <c r="C10" s="15" t="s">
+        <v>16</v>
+      </c>
+      <c r="D10" s="15" t="s">
+        <v>16</v>
+      </c>
+      <c r="E10" s="16" t="s">
+        <v>20</v>
+      </c>
+      <c r="F10" s="15" t="s">
+        <v>16</v>
+      </c>
+      <c r="G10" s="15" t="s">
+        <v>16</v>
+      </c>
+      <c r="H10" s="15" t="s">
+        <v>16</v>
+      </c>
+      <c r="I10" s="16" t="s">
+        <v>20</v>
+      </c>
+      <c r="J10" s="15" t="s">
+        <v>16</v>
+      </c>
+      <c r="K10" s="16" t="s">
+        <v>20</v>
+      </c>
+      <c r="L10" s="15" t="s">
+        <v>16</v>
       </c>
       <c r="M10" s="2">
         <v>9</v>
@@ -2251,38 +2384,38 @@
       <c r="A11" s="2">
         <v>1</v>
       </c>
-      <c r="B11" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="C11" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="D11" s="2" t="s">
-        <v>41</v>
-      </c>
-      <c r="E11" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="F11" s="4" t="s">
-        <v>39</v>
-      </c>
-      <c r="G11" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="H11" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="I11" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="J11" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="K11" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="L11" s="2" t="s">
-        <v>39</v>
+      <c r="B11" s="14" t="s">
+        <v>16</v>
+      </c>
+      <c r="C11" s="15" t="s">
+        <v>16</v>
+      </c>
+      <c r="D11" s="16" t="s">
+        <v>22</v>
+      </c>
+      <c r="E11" s="15" t="s">
+        <v>16</v>
+      </c>
+      <c r="F11" s="15" t="s">
+        <v>16</v>
+      </c>
+      <c r="G11" s="15" t="s">
+        <v>16</v>
+      </c>
+      <c r="H11" s="16" t="s">
+        <v>22</v>
+      </c>
+      <c r="I11" s="15" t="s">
+        <v>16</v>
+      </c>
+      <c r="J11" s="15" t="s">
+        <v>16</v>
+      </c>
+      <c r="K11" s="15" t="s">
+        <v>16</v>
+      </c>
+      <c r="L11" s="16" t="s">
+        <v>22</v>
       </c>
       <c r="M11" s="2">
         <v>10</v>
@@ -2293,38 +2426,38 @@
       <c r="A12" s="2">
         <v>1</v>
       </c>
-      <c r="B12" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="C12" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="D12" s="2" t="s">
-        <v>41</v>
-      </c>
-      <c r="E12" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="F12" s="4" t="s">
-        <v>39</v>
-      </c>
-      <c r="G12" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="H12" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="I12" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="J12" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="K12" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="L12" s="2" t="s">
-        <v>39</v>
+      <c r="B12" s="14" t="s">
+        <v>16</v>
+      </c>
+      <c r="C12" s="15" t="s">
+        <v>16</v>
+      </c>
+      <c r="D12" s="15" t="s">
+        <v>16</v>
+      </c>
+      <c r="E12" s="15" t="s">
+        <v>16</v>
+      </c>
+      <c r="F12" s="15" t="s">
+        <v>16</v>
+      </c>
+      <c r="G12" s="11" t="s">
+        <v>21</v>
+      </c>
+      <c r="H12" s="17" t="s">
+        <v>16</v>
+      </c>
+      <c r="I12" s="14" t="s">
+        <v>16</v>
+      </c>
+      <c r="J12" s="15" t="s">
+        <v>16</v>
+      </c>
+      <c r="K12" s="15" t="s">
+        <v>16</v>
+      </c>
+      <c r="L12" s="15" t="s">
+        <v>16</v>
       </c>
       <c r="M12" s="2">
         <v>11</v>
@@ -2372,13 +2505,13 @@
   <mergeCells count="1">
     <mergeCell ref="O2:R7"/>
   </mergeCells>
-  <conditionalFormatting sqref="A14:L1048576 A13:M13 A1:N12">
-    <cfRule type="containsText" dxfId="1" priority="2" operator="containsText" text="{">
+  <conditionalFormatting sqref="A1:N1 A13:M13 A14:L1048576 A2:A12 M2:N12">
+    <cfRule type="containsText" dxfId="3" priority="2" operator="containsText" text="{">
       <formula>NOT(ISERROR(SEARCH("{",A1)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B1:L1048576">
-    <cfRule type="containsText" dxfId="0" priority="1" operator="containsText" text="(">
+  <conditionalFormatting sqref="B1:L1 B13:L1048576">
+    <cfRule type="containsText" dxfId="2" priority="1" operator="containsText" text="(">
       <formula>NOT(ISERROR(SEARCH("(",B1)))</formula>
     </cfRule>
   </conditionalFormatting>
@@ -2389,10 +2522,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{613A7648-F18E-AE44-AC03-528A68E0F000}">
-  <dimension ref="A1:F1"/>
+  <dimension ref="A1:F2"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2423,6 +2556,14 @@
       </c>
       <c r="F1" s="8"/>
     </row>
+    <row r="2" spans="1:6" ht="252" x14ac:dyDescent="0.2">
+      <c r="A2" s="7" t="s">
+        <v>40</v>
+      </c>
+      <c r="B2" s="7" t="s">
+        <v>41</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>

</xml_diff>

<commit_message>
TileControl() Refactor. Change name to TileBag(), Change data structure from HashMap to ArrayList. Create new single Tile() class and tileSetArray(), Refactor tile methods.
</commit_message>
<xml_diff>
--- a/Ancillary Docs/Default Board Helper File.xlsx
+++ b/Ancillary Docs/Default Board Helper File.xlsx
@@ -5,19 +5,20 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/xeon2035/Library/Mobile Documents/com~apple~CloudDocs/UniWerk/SKraBBKle/Ancillary Docs/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/xeon2035/Library/Mobile Documents/com~apple~CloudDocs/UniWerk/13/Ancillary Docs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E0DCCCED-1ABE-BF4B-82D6-E040D982814F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D938FFF1-5DC4-824E-917C-6EE0E81F886E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="60" yWindow="500" windowWidth="26740" windowHeight="14620" activeTab="1" xr2:uid="{F938695B-E880-FB4D-B508-A292FAB83920}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="26740" windowHeight="14620" activeTab="3" xr2:uid="{F938695B-E880-FB4D-B508-A292FAB83920}"/>
   </bookViews>
   <sheets>
     <sheet name="BOARD 16" sheetId="1" r:id="rId1"/>
     <sheet name="BOARD 11" sheetId="3" r:id="rId2"/>
     <sheet name="Test Data" sheetId="2" r:id="rId3"/>
+    <sheet name="Array List Tile Coding" sheetId="4" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -38,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="439" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="654" uniqueCount="110">
   <si>
     <t>a</t>
   </si>
@@ -267,12 +268,219 @@
 .(3)...(3)...(3).
 {2}.....{2}....</t>
   </si>
+  <si>
+    <t>x</t>
+  </si>
+  <si>
+    <t>[A1]</t>
+  </si>
+  <si>
+    <t>[B3]</t>
+  </si>
+  <si>
+    <t>[C3]</t>
+  </si>
+  <si>
+    <t>[D2]</t>
+  </si>
+  <si>
+    <t>[E1]</t>
+  </si>
+  <si>
+    <t>[F4]</t>
+  </si>
+  <si>
+    <t>[G2]</t>
+  </si>
+  <si>
+    <t>[H4]</t>
+  </si>
+  <si>
+    <t>[I1]</t>
+  </si>
+  <si>
+    <t>[J9]</t>
+  </si>
+  <si>
+    <t>[K6]</t>
+  </si>
+  <si>
+    <t>[L1]</t>
+  </si>
+  <si>
+    <t>[M3]</t>
+  </si>
+  <si>
+    <t>[N1]</t>
+  </si>
+  <si>
+    <t>[O1]</t>
+  </si>
+  <si>
+    <t>[P3]</t>
+  </si>
+  <si>
+    <t>[Q12]</t>
+  </si>
+  <si>
+    <t>[R1]</t>
+  </si>
+  <si>
+    <t>[S1]</t>
+  </si>
+  <si>
+    <t>[T1]</t>
+  </si>
+  <si>
+    <t>[U1]</t>
+  </si>
+  <si>
+    <t>[V4]</t>
+  </si>
+  <si>
+    <t>[W4]</t>
+  </si>
+  <si>
+    <t>[X9]</t>
+  </si>
+  <si>
+    <t>[Y5]</t>
+  </si>
+  <si>
+    <t>[Z11]</t>
+  </si>
+  <si>
+    <t>A</t>
+  </si>
+  <si>
+    <t>1</t>
+  </si>
+  <si>
+    <t>B</t>
+  </si>
+  <si>
+    <t>3</t>
+  </si>
+  <si>
+    <t>C</t>
+  </si>
+  <si>
+    <t>D</t>
+  </si>
+  <si>
+    <t>2</t>
+  </si>
+  <si>
+    <t>E</t>
+  </si>
+  <si>
+    <t>F</t>
+  </si>
+  <si>
+    <t>4</t>
+  </si>
+  <si>
+    <t>G</t>
+  </si>
+  <si>
+    <t>H</t>
+  </si>
+  <si>
+    <t>I</t>
+  </si>
+  <si>
+    <t>J</t>
+  </si>
+  <si>
+    <t>9</t>
+  </si>
+  <si>
+    <t>K</t>
+  </si>
+  <si>
+    <t>6</t>
+  </si>
+  <si>
+    <t>L</t>
+  </si>
+  <si>
+    <t>M</t>
+  </si>
+  <si>
+    <t>N</t>
+  </si>
+  <si>
+    <t>O</t>
+  </si>
+  <si>
+    <t>P</t>
+  </si>
+  <si>
+    <t>Q</t>
+  </si>
+  <si>
+    <t>12</t>
+  </si>
+  <si>
+    <t>R</t>
+  </si>
+  <si>
+    <t>S</t>
+  </si>
+  <si>
+    <t>T</t>
+  </si>
+  <si>
+    <t>U</t>
+  </si>
+  <si>
+    <t>V</t>
+  </si>
+  <si>
+    <t>W</t>
+  </si>
+  <si>
+    <t>X</t>
+  </si>
+  <si>
+    <t>Y</t>
+  </si>
+  <si>
+    <t>5</t>
+  </si>
+  <si>
+    <t>Z</t>
+  </si>
+  <si>
+    <t>11</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> for (int i = 0; i &lt;</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> ; i++) {
+            tileSet.add(new Tile('</t>
+  </si>
+  <si>
+    <t xml:space="preserve">, </t>
+  </si>
+  <si>
+    <t xml:space="preserve">));
+        }
+        </t>
+  </si>
+  <si>
+    <t>_</t>
+  </si>
+  <si>
+    <t>[_5]</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -304,6 +512,25 @@
     <font>
       <sz val="12"/>
       <color rgb="FF000000"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="15"/>
+      <color theme="1"/>
+      <name val="Helvetica"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="15"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="15"/>
+      <color rgb="FFFF0000"/>
       <name val="Aptos Narrow"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -393,7 +620,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -419,9 +646,6 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="49" fontId="4" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -446,31 +670,32 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="6">
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="4">
     <dxf>
       <font>
         <color rgb="FF006100"/>
@@ -964,12 +1189,12 @@
         <v>1</v>
       </c>
       <c r="S2" s="3"/>
-      <c r="T2" s="9" t="s">
+      <c r="T2" s="23" t="s">
         <v>33</v>
       </c>
-      <c r="U2" s="9"/>
-      <c r="V2" s="9"/>
-      <c r="W2" s="9"/>
+      <c r="U2" s="23"/>
+      <c r="V2" s="23"/>
+      <c r="W2" s="23"/>
     </row>
     <row r="3" spans="1:23" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="2">
@@ -1027,10 +1252,10 @@
         <v>2</v>
       </c>
       <c r="S3" s="3"/>
-      <c r="T3" s="9"/>
-      <c r="U3" s="9"/>
-      <c r="V3" s="9"/>
-      <c r="W3" s="9"/>
+      <c r="T3" s="23"/>
+      <c r="U3" s="23"/>
+      <c r="V3" s="23"/>
+      <c r="W3" s="23"/>
     </row>
     <row r="4" spans="1:23" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="2">
@@ -1088,10 +1313,10 @@
         <v>3</v>
       </c>
       <c r="S4" s="3"/>
-      <c r="T4" s="9"/>
-      <c r="U4" s="9"/>
-      <c r="V4" s="9"/>
-      <c r="W4" s="9"/>
+      <c r="T4" s="23"/>
+      <c r="U4" s="23"/>
+      <c r="V4" s="23"/>
+      <c r="W4" s="23"/>
     </row>
     <row r="5" spans="1:23" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="2">
@@ -1149,10 +1374,10 @@
         <v>4</v>
       </c>
       <c r="S5" s="3"/>
-      <c r="T5" s="9"/>
-      <c r="U5" s="9"/>
-      <c r="V5" s="9"/>
-      <c r="W5" s="9"/>
+      <c r="T5" s="23"/>
+      <c r="U5" s="23"/>
+      <c r="V5" s="23"/>
+      <c r="W5" s="23"/>
     </row>
     <row r="6" spans="1:23" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="2">
@@ -1210,10 +1435,10 @@
         <v>5</v>
       </c>
       <c r="S6" s="3"/>
-      <c r="T6" s="9"/>
-      <c r="U6" s="9"/>
-      <c r="V6" s="9"/>
-      <c r="W6" s="9"/>
+      <c r="T6" s="23"/>
+      <c r="U6" s="23"/>
+      <c r="V6" s="23"/>
+      <c r="W6" s="23"/>
     </row>
     <row r="7" spans="1:23" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="2">
@@ -1271,10 +1496,10 @@
         <v>6</v>
       </c>
       <c r="S7" s="3"/>
-      <c r="T7" s="9"/>
-      <c r="U7" s="9"/>
-      <c r="V7" s="9"/>
-      <c r="W7" s="9"/>
+      <c r="T7" s="23"/>
+      <c r="U7" s="23"/>
+      <c r="V7" s="23"/>
+      <c r="W7" s="23"/>
     </row>
     <row r="8" spans="1:23" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="2">
@@ -1904,12 +2129,12 @@
     <mergeCell ref="T2:W7"/>
   </mergeCells>
   <conditionalFormatting sqref="A1:Q11 A12:G12 I12:Q12 A13:Q17 A18:R18 A19:Q1048576 R1:S17">
-    <cfRule type="containsText" dxfId="5" priority="2" operator="containsText" text="{">
+    <cfRule type="containsText" dxfId="3" priority="2" operator="containsText" text="{">
       <formula>NOT(ISERROR(SEARCH("{",A1)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B1:Q11 B12:G12 I12:Q12 B13:Q1048576">
-    <cfRule type="containsText" dxfId="4" priority="1" operator="containsText" text="(">
+    <cfRule type="containsText" dxfId="2" priority="1" operator="containsText" text="(">
       <formula>NOT(ISERROR(SEARCH("(",B1)))</formula>
     </cfRule>
   </conditionalFormatting>
@@ -1925,9 +2150,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6BAE5677-87B1-5C4F-AA9E-8B56D72F0A3D}">
   <dimension ref="A1:R13"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+    <sheetView showGridLines="0" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B2" sqref="B2:L12"/>
+      <selection pane="bottomLeft" activeCell="N7" sqref="N7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="19" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1979,315 +2204,315 @@
       <c r="A2" s="2">
         <v>1</v>
       </c>
-      <c r="B2" s="10" t="s">
-        <v>16</v>
-      </c>
-      <c r="C2" s="11" t="s">
+      <c r="B2" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="C2" s="10" t="s">
         <v>17</v>
       </c>
-      <c r="D2" s="12" t="s">
-        <v>16</v>
-      </c>
-      <c r="E2" s="12" t="s">
-        <v>16</v>
-      </c>
-      <c r="F2" s="13">
+      <c r="D2" s="11" t="s">
+        <v>16</v>
+      </c>
+      <c r="E2" s="11" t="s">
+        <v>16</v>
+      </c>
+      <c r="F2" s="12">
         <v>-2</v>
       </c>
-      <c r="G2" s="12" t="s">
-        <v>16</v>
-      </c>
-      <c r="H2" s="12" t="s">
-        <v>16</v>
-      </c>
-      <c r="I2" s="12" t="s">
-        <v>16</v>
-      </c>
-      <c r="J2" s="11" t="s">
+      <c r="G2" s="11" t="s">
+        <v>16</v>
+      </c>
+      <c r="H2" s="11" t="s">
+        <v>16</v>
+      </c>
+      <c r="I2" s="11" t="s">
+        <v>16</v>
+      </c>
+      <c r="J2" s="10" t="s">
         <v>18</v>
       </c>
-      <c r="K2" s="12" t="s">
-        <v>16</v>
-      </c>
-      <c r="L2" s="12" t="s">
+      <c r="K2" s="11" t="s">
+        <v>16</v>
+      </c>
+      <c r="L2" s="11" t="s">
         <v>16</v>
       </c>
       <c r="M2" s="2">
         <v>1</v>
       </c>
       <c r="N2" s="3"/>
-      <c r="O2" s="9" t="s">
+      <c r="O2" s="23" t="s">
         <v>39</v>
       </c>
-      <c r="P2" s="9"/>
-      <c r="Q2" s="9"/>
-      <c r="R2" s="9"/>
+      <c r="P2" s="23"/>
+      <c r="Q2" s="23"/>
+      <c r="R2" s="23"/>
     </row>
     <row r="3" spans="1:18" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="2">
         <v>1</v>
       </c>
-      <c r="B3" s="14" t="s">
-        <v>16</v>
-      </c>
-      <c r="C3" s="15" t="s">
-        <v>16</v>
-      </c>
-      <c r="D3" s="11" t="s">
+      <c r="B3" s="13" t="s">
+        <v>16</v>
+      </c>
+      <c r="C3" s="14" t="s">
+        <v>16</v>
+      </c>
+      <c r="D3" s="10" t="s">
         <v>21</v>
       </c>
-      <c r="E3" s="15" t="s">
-        <v>16</v>
-      </c>
-      <c r="F3" s="15" t="s">
-        <v>16</v>
-      </c>
-      <c r="G3" s="15" t="s">
-        <v>16</v>
-      </c>
-      <c r="H3" s="16" t="s">
+      <c r="E3" s="14" t="s">
+        <v>16</v>
+      </c>
+      <c r="F3" s="14" t="s">
+        <v>16</v>
+      </c>
+      <c r="G3" s="14" t="s">
+        <v>16</v>
+      </c>
+      <c r="H3" s="15" t="s">
         <v>22</v>
       </c>
-      <c r="I3" s="15" t="s">
-        <v>16</v>
-      </c>
-      <c r="J3" s="15" t="s">
-        <v>16</v>
-      </c>
-      <c r="K3" s="15" t="s">
-        <v>16</v>
-      </c>
-      <c r="L3" s="16" t="s">
+      <c r="I3" s="14" t="s">
+        <v>16</v>
+      </c>
+      <c r="J3" s="14" t="s">
+        <v>16</v>
+      </c>
+      <c r="K3" s="14" t="s">
+        <v>16</v>
+      </c>
+      <c r="L3" s="15" t="s">
         <v>22</v>
       </c>
       <c r="M3" s="2">
         <v>2</v>
       </c>
       <c r="N3" s="3"/>
-      <c r="O3" s="9"/>
-      <c r="P3" s="9"/>
-      <c r="Q3" s="9"/>
-      <c r="R3" s="9"/>
+      <c r="O3" s="23"/>
+      <c r="P3" s="23"/>
+      <c r="Q3" s="23"/>
+      <c r="R3" s="23"/>
     </row>
     <row r="4" spans="1:18" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="2">
         <v>1</v>
       </c>
-      <c r="B4" s="14" t="s">
-        <v>16</v>
-      </c>
-      <c r="C4" s="15" t="s">
-        <v>16</v>
-      </c>
-      <c r="D4" s="15" t="s">
-        <v>16</v>
-      </c>
-      <c r="E4" s="11" t="s">
+      <c r="B4" s="13" t="s">
+        <v>16</v>
+      </c>
+      <c r="C4" s="14" t="s">
+        <v>16</v>
+      </c>
+      <c r="D4" s="14" t="s">
+        <v>16</v>
+      </c>
+      <c r="E4" s="10" t="s">
         <v>21</v>
       </c>
-      <c r="F4" s="15" t="s">
-        <v>16</v>
-      </c>
-      <c r="G4" s="15" t="s">
-        <v>16</v>
-      </c>
-      <c r="H4" s="15" t="s">
-        <v>16</v>
-      </c>
-      <c r="I4" s="16" t="s">
+      <c r="F4" s="14" t="s">
+        <v>16</v>
+      </c>
+      <c r="G4" s="14" t="s">
+        <v>16</v>
+      </c>
+      <c r="H4" s="14" t="s">
+        <v>16</v>
+      </c>
+      <c r="I4" s="15" t="s">
         <v>20</v>
       </c>
-      <c r="J4" s="15" t="s">
-        <v>16</v>
-      </c>
-      <c r="K4" s="16" t="s">
+      <c r="J4" s="14" t="s">
+        <v>16</v>
+      </c>
+      <c r="K4" s="15" t="s">
         <v>20</v>
       </c>
-      <c r="L4" s="15" t="s">
+      <c r="L4" s="14" t="s">
         <v>16</v>
       </c>
       <c r="M4" s="2">
         <v>3</v>
       </c>
       <c r="N4" s="3"/>
-      <c r="O4" s="9"/>
-      <c r="P4" s="9"/>
-      <c r="Q4" s="9"/>
-      <c r="R4" s="9"/>
+      <c r="O4" s="23"/>
+      <c r="P4" s="23"/>
+      <c r="Q4" s="23"/>
+      <c r="R4" s="23"/>
     </row>
     <row r="5" spans="1:18" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="2">
         <v>1</v>
       </c>
-      <c r="B5" s="14" t="s">
-        <v>16</v>
-      </c>
-      <c r="C5" s="16" t="s">
+      <c r="B5" s="13" t="s">
+        <v>16</v>
+      </c>
+      <c r="C5" s="15" t="s">
         <v>20</v>
       </c>
-      <c r="D5" s="15" t="s">
-        <v>16</v>
-      </c>
-      <c r="E5" s="15" t="s">
-        <v>16</v>
-      </c>
-      <c r="F5" s="11" t="s">
+      <c r="D5" s="14" t="s">
+        <v>16</v>
+      </c>
+      <c r="E5" s="14" t="s">
+        <v>16</v>
+      </c>
+      <c r="F5" s="10" t="s">
         <v>21</v>
       </c>
-      <c r="G5" s="15" t="s">
-        <v>16</v>
-      </c>
-      <c r="H5" s="15" t="s">
-        <v>16</v>
-      </c>
-      <c r="I5" s="15" t="s">
-        <v>16</v>
-      </c>
-      <c r="J5" s="16" t="s">
+      <c r="G5" s="14" t="s">
+        <v>16</v>
+      </c>
+      <c r="H5" s="14" t="s">
+        <v>16</v>
+      </c>
+      <c r="I5" s="14" t="s">
+        <v>16</v>
+      </c>
+      <c r="J5" s="15" t="s">
         <v>20</v>
       </c>
-      <c r="K5" s="15" t="s">
-        <v>16</v>
-      </c>
-      <c r="L5" s="15" t="s">
+      <c r="K5" s="14" t="s">
+        <v>16</v>
+      </c>
+      <c r="L5" s="14" t="s">
         <v>16</v>
       </c>
       <c r="M5" s="2">
         <v>4</v>
       </c>
       <c r="N5" s="3"/>
-      <c r="O5" s="9"/>
-      <c r="P5" s="9"/>
-      <c r="Q5" s="9"/>
-      <c r="R5" s="9"/>
+      <c r="O5" s="23"/>
+      <c r="P5" s="23"/>
+      <c r="Q5" s="23"/>
+      <c r="R5" s="23"/>
     </row>
     <row r="6" spans="1:18" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="2">
         <v>1</v>
       </c>
-      <c r="B6" s="14" t="s">
-        <v>16</v>
-      </c>
-      <c r="C6" s="15" t="s">
-        <v>16</v>
-      </c>
-      <c r="D6" s="15" t="s">
-        <v>16</v>
-      </c>
-      <c r="E6" s="15" t="s">
-        <v>16</v>
-      </c>
-      <c r="F6" s="15" t="s">
-        <v>16</v>
-      </c>
-      <c r="G6" s="11" t="s">
+      <c r="B6" s="13" t="s">
+        <v>16</v>
+      </c>
+      <c r="C6" s="14" t="s">
+        <v>16</v>
+      </c>
+      <c r="D6" s="14" t="s">
+        <v>16</v>
+      </c>
+      <c r="E6" s="14" t="s">
+        <v>16</v>
+      </c>
+      <c r="F6" s="14" t="s">
+        <v>16</v>
+      </c>
+      <c r="G6" s="10" t="s">
         <v>21</v>
       </c>
-      <c r="H6" s="15" t="s">
-        <v>16</v>
-      </c>
-      <c r="I6" s="15" t="s">
-        <v>16</v>
-      </c>
-      <c r="J6" s="15" t="s">
-        <v>16</v>
-      </c>
-      <c r="K6" s="15" t="s">
-        <v>16</v>
-      </c>
-      <c r="L6" s="15" t="s">
+      <c r="H6" s="14" t="s">
+        <v>16</v>
+      </c>
+      <c r="I6" s="14" t="s">
+        <v>16</v>
+      </c>
+      <c r="J6" s="14" t="s">
+        <v>16</v>
+      </c>
+      <c r="K6" s="14" t="s">
+        <v>16</v>
+      </c>
+      <c r="L6" s="14" t="s">
         <v>16</v>
       </c>
       <c r="M6" s="2">
         <v>5</v>
       </c>
       <c r="N6" s="3"/>
-      <c r="O6" s="9"/>
-      <c r="P6" s="9"/>
-      <c r="Q6" s="9"/>
-      <c r="R6" s="9"/>
+      <c r="O6" s="23"/>
+      <c r="P6" s="23"/>
+      <c r="Q6" s="23"/>
+      <c r="R6" s="23"/>
     </row>
     <row r="7" spans="1:18" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="2">
         <v>1</v>
       </c>
-      <c r="B7" s="14" t="s">
-        <v>16</v>
-      </c>
-      <c r="C7" s="15" t="s">
-        <v>16</v>
-      </c>
-      <c r="D7" s="16" t="s">
+      <c r="B7" s="13" t="s">
+        <v>16</v>
+      </c>
+      <c r="C7" s="14" t="s">
+        <v>16</v>
+      </c>
+      <c r="D7" s="15" t="s">
         <v>22</v>
       </c>
-      <c r="E7" s="15" t="s">
-        <v>16</v>
-      </c>
-      <c r="F7" s="15" t="s">
-        <v>16</v>
-      </c>
-      <c r="G7" s="15" t="s">
-        <v>16</v>
-      </c>
-      <c r="H7" s="16" t="s">
+      <c r="E7" s="14" t="s">
+        <v>16</v>
+      </c>
+      <c r="F7" s="14" t="s">
+        <v>16</v>
+      </c>
+      <c r="G7" s="14" t="s">
+        <v>16</v>
+      </c>
+      <c r="H7" s="15" t="s">
         <v>22</v>
       </c>
-      <c r="I7" s="15" t="s">
-        <v>16</v>
-      </c>
-      <c r="J7" s="15" t="s">
-        <v>16</v>
-      </c>
-      <c r="K7" s="15" t="s">
-        <v>16</v>
-      </c>
-      <c r="L7" s="16" t="s">
+      <c r="I7" s="14" t="s">
+        <v>16</v>
+      </c>
+      <c r="J7" s="14" t="s">
+        <v>16</v>
+      </c>
+      <c r="K7" s="14" t="s">
+        <v>16</v>
+      </c>
+      <c r="L7" s="15" t="s">
         <v>22</v>
       </c>
       <c r="M7" s="2">
         <v>6</v>
       </c>
       <c r="N7" s="3"/>
-      <c r="O7" s="9"/>
-      <c r="P7" s="9"/>
-      <c r="Q7" s="9"/>
-      <c r="R7" s="9"/>
+      <c r="O7" s="23"/>
+      <c r="P7" s="23"/>
+      <c r="Q7" s="23"/>
+      <c r="R7" s="23"/>
     </row>
     <row r="8" spans="1:18" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="2">
         <v>1</v>
       </c>
-      <c r="B8" s="14" t="s">
-        <v>16</v>
-      </c>
-      <c r="C8" s="15" t="s">
-        <v>16</v>
-      </c>
-      <c r="D8" s="15" t="s">
-        <v>16</v>
-      </c>
-      <c r="E8" s="16" t="s">
+      <c r="B8" s="13" t="s">
+        <v>16</v>
+      </c>
+      <c r="C8" s="14" t="s">
+        <v>16</v>
+      </c>
+      <c r="D8" s="14" t="s">
+        <v>16</v>
+      </c>
+      <c r="E8" s="15" t="s">
         <v>20</v>
       </c>
-      <c r="F8" s="15" t="s">
-        <v>16</v>
-      </c>
-      <c r="G8" s="15" t="s">
-        <v>16</v>
-      </c>
-      <c r="H8" s="15" t="s">
-        <v>16</v>
-      </c>
-      <c r="I8" s="16" t="s">
+      <c r="F8" s="14" t="s">
+        <v>16</v>
+      </c>
+      <c r="G8" s="14" t="s">
+        <v>16</v>
+      </c>
+      <c r="H8" s="14" t="s">
+        <v>16</v>
+      </c>
+      <c r="I8" s="15" t="s">
         <v>20</v>
       </c>
-      <c r="J8" s="15" t="s">
-        <v>16</v>
-      </c>
-      <c r="K8" s="16" t="s">
+      <c r="J8" s="14" t="s">
+        <v>16</v>
+      </c>
+      <c r="K8" s="15" t="s">
         <v>20</v>
       </c>
-      <c r="L8" s="15" t="s">
+      <c r="L8" s="14" t="s">
         <v>16</v>
       </c>
       <c r="M8" s="2">
@@ -2300,37 +2525,37 @@
       <c r="A9" s="2">
         <v>1</v>
       </c>
-      <c r="B9" s="16" t="s">
+      <c r="B9" s="15" t="s">
         <v>22</v>
       </c>
-      <c r="C9" s="11" t="s">
+      <c r="C9" s="10" t="s">
         <v>24</v>
       </c>
-      <c r="D9" s="15" t="s">
-        <v>16</v>
-      </c>
-      <c r="E9" s="15" t="s">
-        <v>16</v>
-      </c>
-      <c r="F9" s="16" t="s">
+      <c r="D9" s="14" t="s">
+        <v>16</v>
+      </c>
+      <c r="E9" s="14" t="s">
+        <v>16</v>
+      </c>
+      <c r="F9" s="15" t="s">
         <v>20</v>
       </c>
-      <c r="G9" s="15" t="s">
-        <v>16</v>
-      </c>
-      <c r="H9" s="15" t="s">
-        <v>16</v>
-      </c>
-      <c r="I9" s="15" t="s">
-        <v>16</v>
-      </c>
-      <c r="J9" s="11" t="s">
+      <c r="G9" s="14" t="s">
+        <v>16</v>
+      </c>
+      <c r="H9" s="14" t="s">
+        <v>16</v>
+      </c>
+      <c r="I9" s="14" t="s">
+        <v>16</v>
+      </c>
+      <c r="J9" s="10" t="s">
         <v>21</v>
       </c>
-      <c r="K9" s="15" t="s">
-        <v>16</v>
-      </c>
-      <c r="L9" s="15" t="s">
+      <c r="K9" s="14" t="s">
+        <v>16</v>
+      </c>
+      <c r="L9" s="14" t="s">
         <v>16</v>
       </c>
       <c r="M9" s="2">
@@ -2342,37 +2567,37 @@
       <c r="A10" s="2">
         <v>1</v>
       </c>
-      <c r="B10" s="14" t="s">
-        <v>16</v>
-      </c>
-      <c r="C10" s="15" t="s">
-        <v>16</v>
-      </c>
-      <c r="D10" s="15" t="s">
-        <v>16</v>
-      </c>
-      <c r="E10" s="16" t="s">
+      <c r="B10" s="13" t="s">
+        <v>16</v>
+      </c>
+      <c r="C10" s="14" t="s">
+        <v>16</v>
+      </c>
+      <c r="D10" s="14" t="s">
+        <v>16</v>
+      </c>
+      <c r="E10" s="15" t="s">
         <v>20</v>
       </c>
-      <c r="F10" s="15" t="s">
-        <v>16</v>
-      </c>
-      <c r="G10" s="15" t="s">
-        <v>16</v>
-      </c>
-      <c r="H10" s="15" t="s">
-        <v>16</v>
-      </c>
-      <c r="I10" s="16" t="s">
+      <c r="F10" s="14" t="s">
+        <v>16</v>
+      </c>
+      <c r="G10" s="14" t="s">
+        <v>16</v>
+      </c>
+      <c r="H10" s="14" t="s">
+        <v>16</v>
+      </c>
+      <c r="I10" s="15" t="s">
         <v>20</v>
       </c>
-      <c r="J10" s="15" t="s">
-        <v>16</v>
-      </c>
-      <c r="K10" s="16" t="s">
+      <c r="J10" s="14" t="s">
+        <v>16</v>
+      </c>
+      <c r="K10" s="15" t="s">
         <v>20</v>
       </c>
-      <c r="L10" s="15" t="s">
+      <c r="L10" s="14" t="s">
         <v>16</v>
       </c>
       <c r="M10" s="2">
@@ -2384,37 +2609,37 @@
       <c r="A11" s="2">
         <v>1</v>
       </c>
-      <c r="B11" s="14" t="s">
-        <v>16</v>
-      </c>
-      <c r="C11" s="15" t="s">
-        <v>16</v>
-      </c>
-      <c r="D11" s="16" t="s">
+      <c r="B11" s="13" t="s">
+        <v>16</v>
+      </c>
+      <c r="C11" s="14" t="s">
+        <v>16</v>
+      </c>
+      <c r="D11" s="15" t="s">
         <v>22</v>
       </c>
-      <c r="E11" s="15" t="s">
-        <v>16</v>
-      </c>
-      <c r="F11" s="15" t="s">
-        <v>16</v>
-      </c>
-      <c r="G11" s="15" t="s">
-        <v>16</v>
-      </c>
-      <c r="H11" s="16" t="s">
+      <c r="E11" s="14" t="s">
+        <v>16</v>
+      </c>
+      <c r="F11" s="14" t="s">
+        <v>16</v>
+      </c>
+      <c r="G11" s="14" t="s">
+        <v>16</v>
+      </c>
+      <c r="H11" s="15" t="s">
         <v>22</v>
       </c>
-      <c r="I11" s="15" t="s">
-        <v>16</v>
-      </c>
-      <c r="J11" s="15" t="s">
-        <v>16</v>
-      </c>
-      <c r="K11" s="15" t="s">
-        <v>16</v>
-      </c>
-      <c r="L11" s="16" t="s">
+      <c r="I11" s="14" t="s">
+        <v>16</v>
+      </c>
+      <c r="J11" s="14" t="s">
+        <v>16</v>
+      </c>
+      <c r="K11" s="14" t="s">
+        <v>16</v>
+      </c>
+      <c r="L11" s="15" t="s">
         <v>22</v>
       </c>
       <c r="M11" s="2">
@@ -2426,37 +2651,37 @@
       <c r="A12" s="2">
         <v>1</v>
       </c>
-      <c r="B12" s="14" t="s">
-        <v>16</v>
-      </c>
-      <c r="C12" s="15" t="s">
-        <v>16</v>
-      </c>
-      <c r="D12" s="15" t="s">
-        <v>16</v>
-      </c>
-      <c r="E12" s="15" t="s">
-        <v>16</v>
-      </c>
-      <c r="F12" s="15" t="s">
-        <v>16</v>
-      </c>
-      <c r="G12" s="11" t="s">
+      <c r="B12" s="13" t="s">
+        <v>16</v>
+      </c>
+      <c r="C12" s="14" t="s">
+        <v>16</v>
+      </c>
+      <c r="D12" s="14" t="s">
+        <v>16</v>
+      </c>
+      <c r="E12" s="14" t="s">
+        <v>16</v>
+      </c>
+      <c r="F12" s="14" t="s">
+        <v>16</v>
+      </c>
+      <c r="G12" s="10" t="s">
         <v>21</v>
       </c>
-      <c r="H12" s="17" t="s">
-        <v>16</v>
-      </c>
-      <c r="I12" s="14" t="s">
-        <v>16</v>
-      </c>
-      <c r="J12" s="15" t="s">
-        <v>16</v>
-      </c>
-      <c r="K12" s="15" t="s">
-        <v>16</v>
-      </c>
-      <c r="L12" s="15" t="s">
+      <c r="H12" s="16" t="s">
+        <v>16</v>
+      </c>
+      <c r="I12" s="13" t="s">
+        <v>16</v>
+      </c>
+      <c r="J12" s="14" t="s">
+        <v>16</v>
+      </c>
+      <c r="K12" s="14" t="s">
+        <v>16</v>
+      </c>
+      <c r="L12" s="14" t="s">
         <v>16</v>
       </c>
       <c r="M12" s="2">
@@ -2506,12 +2731,12 @@
     <mergeCell ref="O2:R7"/>
   </mergeCells>
   <conditionalFormatting sqref="A1:N1 A13:M13 A14:L1048576 A2:A12 M2:N12">
-    <cfRule type="containsText" dxfId="3" priority="2" operator="containsText" text="{">
+    <cfRule type="containsText" dxfId="1" priority="2" operator="containsText" text="{">
       <formula>NOT(ISERROR(SEARCH("{",A1)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B1:L1 B13:L1048576">
-    <cfRule type="containsText" dxfId="2" priority="1" operator="containsText" text="(">
+    <cfRule type="containsText" dxfId="0" priority="1" operator="containsText" text="(">
       <formula>NOT(ISERROR(SEARCH("(",B1)))</formula>
     </cfRule>
   </conditionalFormatting>
@@ -2525,7 +2750,7 @@
   <dimension ref="A1:F2"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2568,4 +2793,1002 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8E2AA095-8C4D-BA40-8955-A2825FB0D37F}">
+  <dimension ref="A1:J27"/>
+  <sheetViews>
+    <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection sqref="A1:A27"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="33" customHeight="1" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="66.83203125" style="22" customWidth="1"/>
+    <col min="2" max="5" width="10.83203125" style="19"/>
+    <col min="6" max="6" width="13.5" style="19" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="19.33203125" style="22" customWidth="1"/>
+    <col min="8" max="8" width="33.5" style="22" customWidth="1"/>
+    <col min="9" max="9" width="8.33203125" style="22" customWidth="1"/>
+    <col min="10" max="10" width="10.83203125" style="22" customWidth="1"/>
+    <col min="11" max="16384" width="10.83203125" style="22"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:10" ht="33" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A1" s="21" t="str">
+        <f t="shared" ref="A1:A27" si="0">G1&amp;F1&amp;H1&amp;B1&amp;"'"&amp;I1&amp;C1&amp;J1</f>
+        <v xml:space="preserve"> for (int i = 0; i &lt;8 ; i++) {
+            tileSet.add(new Tile('A', 1));
+        }
+        </v>
+      </c>
+      <c r="B1" s="19" t="s">
+        <v>69</v>
+      </c>
+      <c r="C1" s="19" t="s">
+        <v>70</v>
+      </c>
+      <c r="D1" s="19" t="s">
+        <v>43</v>
+      </c>
+      <c r="E1" s="19" t="s">
+        <v>42</v>
+      </c>
+      <c r="F1" s="20">
+        <v>8</v>
+      </c>
+      <c r="G1" s="17" t="s">
+        <v>104</v>
+      </c>
+      <c r="H1" s="17" t="s">
+        <v>105</v>
+      </c>
+      <c r="I1" s="18" t="s">
+        <v>106</v>
+      </c>
+      <c r="J1" s="17" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" ht="33" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="21" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> for (int i = 0; i &lt;2 ; i++) {
+            tileSet.add(new Tile('B', 3));
+        }
+        </v>
+      </c>
+      <c r="B2" s="19" t="s">
+        <v>71</v>
+      </c>
+      <c r="C2" s="19" t="s">
+        <v>72</v>
+      </c>
+      <c r="D2" s="19" t="s">
+        <v>44</v>
+      </c>
+      <c r="E2" s="19" t="s">
+        <v>42</v>
+      </c>
+      <c r="F2" s="20">
+        <v>2</v>
+      </c>
+      <c r="G2" s="17" t="s">
+        <v>104</v>
+      </c>
+      <c r="H2" s="17" t="s">
+        <v>105</v>
+      </c>
+      <c r="I2" s="18" t="s">
+        <v>106</v>
+      </c>
+      <c r="J2" s="17" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" ht="33" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A3" s="21" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> for (int i = 0; i &lt;2 ; i++) {
+            tileSet.add(new Tile('C', 3));
+        }
+        </v>
+      </c>
+      <c r="B3" s="19" t="s">
+        <v>73</v>
+      </c>
+      <c r="C3" s="19" t="s">
+        <v>72</v>
+      </c>
+      <c r="D3" s="19" t="s">
+        <v>45</v>
+      </c>
+      <c r="E3" s="19" t="s">
+        <v>42</v>
+      </c>
+      <c r="F3" s="20">
+        <v>2</v>
+      </c>
+      <c r="G3" s="17" t="s">
+        <v>104</v>
+      </c>
+      <c r="H3" s="17" t="s">
+        <v>105</v>
+      </c>
+      <c r="I3" s="18" t="s">
+        <v>106</v>
+      </c>
+      <c r="J3" s="17" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" ht="33" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A4" s="21" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> for (int i = 0; i &lt;4 ; i++) {
+            tileSet.add(new Tile('D', 2));
+        }
+        </v>
+      </c>
+      <c r="B4" s="19" t="s">
+        <v>74</v>
+      </c>
+      <c r="C4" s="19" t="s">
+        <v>75</v>
+      </c>
+      <c r="D4" s="19" t="s">
+        <v>46</v>
+      </c>
+      <c r="E4" s="19" t="s">
+        <v>42</v>
+      </c>
+      <c r="F4" s="20">
+        <v>4</v>
+      </c>
+      <c r="G4" s="17" t="s">
+        <v>104</v>
+      </c>
+      <c r="H4" s="17" t="s">
+        <v>105</v>
+      </c>
+      <c r="I4" s="18" t="s">
+        <v>106</v>
+      </c>
+      <c r="J4" s="17" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" ht="33" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A5" s="21" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> for (int i = 0; i &lt;10 ; i++) {
+            tileSet.add(new Tile('E', 1));
+        }
+        </v>
+      </c>
+      <c r="B5" s="19" t="s">
+        <v>76</v>
+      </c>
+      <c r="C5" s="19" t="s">
+        <v>70</v>
+      </c>
+      <c r="D5" s="19" t="s">
+        <v>47</v>
+      </c>
+      <c r="E5" s="19" t="s">
+        <v>42</v>
+      </c>
+      <c r="F5" s="20">
+        <v>10</v>
+      </c>
+      <c r="G5" s="17" t="s">
+        <v>104</v>
+      </c>
+      <c r="H5" s="17" t="s">
+        <v>105</v>
+      </c>
+      <c r="I5" s="18" t="s">
+        <v>106</v>
+      </c>
+      <c r="J5" s="17" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" ht="33" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A6" s="21" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> for (int i = 0; i &lt;3 ; i++) {
+            tileSet.add(new Tile('F', 4));
+        }
+        </v>
+      </c>
+      <c r="B6" s="19" t="s">
+        <v>77</v>
+      </c>
+      <c r="C6" s="19" t="s">
+        <v>78</v>
+      </c>
+      <c r="D6" s="19" t="s">
+        <v>48</v>
+      </c>
+      <c r="E6" s="19" t="s">
+        <v>42</v>
+      </c>
+      <c r="F6" s="20">
+        <v>3</v>
+      </c>
+      <c r="G6" s="17" t="s">
+        <v>104</v>
+      </c>
+      <c r="H6" s="17" t="s">
+        <v>105</v>
+      </c>
+      <c r="I6" s="18" t="s">
+        <v>106</v>
+      </c>
+      <c r="J6" s="17" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" ht="33" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A7" s="21" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> for (int i = 0; i &lt;4 ; i++) {
+            tileSet.add(new Tile('G', 2));
+        }
+        </v>
+      </c>
+      <c r="B7" s="19" t="s">
+        <v>79</v>
+      </c>
+      <c r="C7" s="19" t="s">
+        <v>75</v>
+      </c>
+      <c r="D7" s="19" t="s">
+        <v>49</v>
+      </c>
+      <c r="E7" s="19" t="s">
+        <v>42</v>
+      </c>
+      <c r="F7" s="20">
+        <v>4</v>
+      </c>
+      <c r="G7" s="17" t="s">
+        <v>104</v>
+      </c>
+      <c r="H7" s="17" t="s">
+        <v>105</v>
+      </c>
+      <c r="I7" s="18" t="s">
+        <v>106</v>
+      </c>
+      <c r="J7" s="17" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" ht="33" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A8" s="21" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> for (int i = 0; i &lt;3 ; i++) {
+            tileSet.add(new Tile('H', 4));
+        }
+        </v>
+      </c>
+      <c r="B8" s="19" t="s">
+        <v>80</v>
+      </c>
+      <c r="C8" s="19" t="s">
+        <v>78</v>
+      </c>
+      <c r="D8" s="19" t="s">
+        <v>50</v>
+      </c>
+      <c r="E8" s="19" t="s">
+        <v>42</v>
+      </c>
+      <c r="F8" s="20">
+        <v>3</v>
+      </c>
+      <c r="G8" s="17" t="s">
+        <v>104</v>
+      </c>
+      <c r="H8" s="17" t="s">
+        <v>105</v>
+      </c>
+      <c r="I8" s="18" t="s">
+        <v>106</v>
+      </c>
+      <c r="J8" s="17" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" ht="33" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A9" s="21" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> for (int i = 0; i &lt;8 ; i++) {
+            tileSet.add(new Tile('I', 1));
+        }
+        </v>
+      </c>
+      <c r="B9" s="19" t="s">
+        <v>81</v>
+      </c>
+      <c r="C9" s="19" t="s">
+        <v>70</v>
+      </c>
+      <c r="D9" s="19" t="s">
+        <v>51</v>
+      </c>
+      <c r="E9" s="19" t="s">
+        <v>42</v>
+      </c>
+      <c r="F9" s="20">
+        <v>8</v>
+      </c>
+      <c r="G9" s="17" t="s">
+        <v>104</v>
+      </c>
+      <c r="H9" s="17" t="s">
+        <v>105</v>
+      </c>
+      <c r="I9" s="18" t="s">
+        <v>106</v>
+      </c>
+      <c r="J9" s="17" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" ht="33" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A10" s="21" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> for (int i = 0; i &lt;1 ; i++) {
+            tileSet.add(new Tile('J', 9));
+        }
+        </v>
+      </c>
+      <c r="B10" s="19" t="s">
+        <v>82</v>
+      </c>
+      <c r="C10" s="19" t="s">
+        <v>83</v>
+      </c>
+      <c r="D10" s="19" t="s">
+        <v>52</v>
+      </c>
+      <c r="E10" s="19" t="s">
+        <v>42</v>
+      </c>
+      <c r="F10" s="20">
+        <v>1</v>
+      </c>
+      <c r="G10" s="17" t="s">
+        <v>104</v>
+      </c>
+      <c r="H10" s="17" t="s">
+        <v>105</v>
+      </c>
+      <c r="I10" s="18" t="s">
+        <v>106</v>
+      </c>
+      <c r="J10" s="17" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" ht="33" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A11" s="21" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> for (int i = 0; i &lt;1 ; i++) {
+            tileSet.add(new Tile('K', 6));
+        }
+        </v>
+      </c>
+      <c r="B11" s="19" t="s">
+        <v>84</v>
+      </c>
+      <c r="C11" s="19" t="s">
+        <v>85</v>
+      </c>
+      <c r="D11" s="19" t="s">
+        <v>53</v>
+      </c>
+      <c r="E11" s="19" t="s">
+        <v>42</v>
+      </c>
+      <c r="F11" s="20">
+        <v>1</v>
+      </c>
+      <c r="G11" s="17" t="s">
+        <v>104</v>
+      </c>
+      <c r="H11" s="17" t="s">
+        <v>105</v>
+      </c>
+      <c r="I11" s="18" t="s">
+        <v>106</v>
+      </c>
+      <c r="J11" s="17" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" ht="33" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A12" s="21" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> for (int i = 0; i &lt;4 ; i++) {
+            tileSet.add(new Tile('L', 1));
+        }
+        </v>
+      </c>
+      <c r="B12" s="19" t="s">
+        <v>86</v>
+      </c>
+      <c r="C12" s="19" t="s">
+        <v>70</v>
+      </c>
+      <c r="D12" s="19" t="s">
+        <v>54</v>
+      </c>
+      <c r="E12" s="19" t="s">
+        <v>42</v>
+      </c>
+      <c r="F12" s="20">
+        <v>4</v>
+      </c>
+      <c r="G12" s="17" t="s">
+        <v>104</v>
+      </c>
+      <c r="H12" s="17" t="s">
+        <v>105</v>
+      </c>
+      <c r="I12" s="18" t="s">
+        <v>106</v>
+      </c>
+      <c r="J12" s="17" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" ht="33" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A13" s="21" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> for (int i = 0; i &lt;2 ; i++) {
+            tileSet.add(new Tile('M', 3));
+        }
+        </v>
+      </c>
+      <c r="B13" s="19" t="s">
+        <v>87</v>
+      </c>
+      <c r="C13" s="19" t="s">
+        <v>72</v>
+      </c>
+      <c r="D13" s="19" t="s">
+        <v>55</v>
+      </c>
+      <c r="E13" s="19" t="s">
+        <v>42</v>
+      </c>
+      <c r="F13" s="20">
+        <v>2</v>
+      </c>
+      <c r="G13" s="17" t="s">
+        <v>104</v>
+      </c>
+      <c r="H13" s="17" t="s">
+        <v>105</v>
+      </c>
+      <c r="I13" s="18" t="s">
+        <v>106</v>
+      </c>
+      <c r="J13" s="17" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" ht="33" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A14" s="21" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> for (int i = 0; i &lt;7 ; i++) {
+            tileSet.add(new Tile('N', 1));
+        }
+        </v>
+      </c>
+      <c r="B14" s="19" t="s">
+        <v>88</v>
+      </c>
+      <c r="C14" s="19" t="s">
+        <v>70</v>
+      </c>
+      <c r="D14" s="19" t="s">
+        <v>56</v>
+      </c>
+      <c r="E14" s="19" t="s">
+        <v>42</v>
+      </c>
+      <c r="F14" s="20">
+        <v>7</v>
+      </c>
+      <c r="G14" s="17" t="s">
+        <v>104</v>
+      </c>
+      <c r="H14" s="17" t="s">
+        <v>105</v>
+      </c>
+      <c r="I14" s="18" t="s">
+        <v>106</v>
+      </c>
+      <c r="J14" s="17" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" ht="33" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A15" s="21" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> for (int i = 0; i &lt;7 ; i++) {
+            tileSet.add(new Tile('O', 1));
+        }
+        </v>
+      </c>
+      <c r="B15" s="19" t="s">
+        <v>89</v>
+      </c>
+      <c r="C15" s="19" t="s">
+        <v>70</v>
+      </c>
+      <c r="D15" s="19" t="s">
+        <v>57</v>
+      </c>
+      <c r="E15" s="19" t="s">
+        <v>42</v>
+      </c>
+      <c r="F15" s="20">
+        <v>7</v>
+      </c>
+      <c r="G15" s="17" t="s">
+        <v>104</v>
+      </c>
+      <c r="H15" s="17" t="s">
+        <v>105</v>
+      </c>
+      <c r="I15" s="18" t="s">
+        <v>106</v>
+      </c>
+      <c r="J15" s="17" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" ht="33" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A16" s="21" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> for (int i = 0; i &lt;2 ; i++) {
+            tileSet.add(new Tile('P', 3));
+        }
+        </v>
+      </c>
+      <c r="B16" s="19" t="s">
+        <v>90</v>
+      </c>
+      <c r="C16" s="19" t="s">
+        <v>72</v>
+      </c>
+      <c r="D16" s="19" t="s">
+        <v>58</v>
+      </c>
+      <c r="E16" s="19" t="s">
+        <v>42</v>
+      </c>
+      <c r="F16" s="20">
+        <v>2</v>
+      </c>
+      <c r="G16" s="17" t="s">
+        <v>104</v>
+      </c>
+      <c r="H16" s="17" t="s">
+        <v>105</v>
+      </c>
+      <c r="I16" s="18" t="s">
+        <v>106</v>
+      </c>
+      <c r="J16" s="17" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10" ht="33" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A17" s="21" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> for (int i = 0; i &lt;1 ; i++) {
+            tileSet.add(new Tile('Q', 12));
+        }
+        </v>
+      </c>
+      <c r="B17" s="19" t="s">
+        <v>91</v>
+      </c>
+      <c r="C17" s="19" t="s">
+        <v>92</v>
+      </c>
+      <c r="D17" s="19" t="s">
+        <v>59</v>
+      </c>
+      <c r="E17" s="19" t="s">
+        <v>42</v>
+      </c>
+      <c r="F17" s="20">
+        <v>1</v>
+      </c>
+      <c r="G17" s="17" t="s">
+        <v>104</v>
+      </c>
+      <c r="H17" s="17" t="s">
+        <v>105</v>
+      </c>
+      <c r="I17" s="18" t="s">
+        <v>106</v>
+      </c>
+      <c r="J17" s="17" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10" ht="33" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A18" s="21" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> for (int i = 0; i &lt;6 ; i++) {
+            tileSet.add(new Tile('R', 1));
+        }
+        </v>
+      </c>
+      <c r="B18" s="19" t="s">
+        <v>93</v>
+      </c>
+      <c r="C18" s="19" t="s">
+        <v>70</v>
+      </c>
+      <c r="D18" s="19" t="s">
+        <v>60</v>
+      </c>
+      <c r="E18" s="19" t="s">
+        <v>42</v>
+      </c>
+      <c r="F18" s="20">
+        <v>6</v>
+      </c>
+      <c r="G18" s="17" t="s">
+        <v>104</v>
+      </c>
+      <c r="H18" s="17" t="s">
+        <v>105</v>
+      </c>
+      <c r="I18" s="18" t="s">
+        <v>106</v>
+      </c>
+      <c r="J18" s="17" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10" ht="33" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A19" s="21" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> for (int i = 0; i &lt;4 ; i++) {
+            tileSet.add(new Tile('S', 1));
+        }
+        </v>
+      </c>
+      <c r="B19" s="19" t="s">
+        <v>94</v>
+      </c>
+      <c r="C19" s="19" t="s">
+        <v>70</v>
+      </c>
+      <c r="D19" s="19" t="s">
+        <v>61</v>
+      </c>
+      <c r="E19" s="19" t="s">
+        <v>42</v>
+      </c>
+      <c r="F19" s="20">
+        <v>4</v>
+      </c>
+      <c r="G19" s="17" t="s">
+        <v>104</v>
+      </c>
+      <c r="H19" s="17" t="s">
+        <v>105</v>
+      </c>
+      <c r="I19" s="18" t="s">
+        <v>106</v>
+      </c>
+      <c r="J19" s="17" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="20" spans="1:10" ht="33" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A20" s="21" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> for (int i = 0; i &lt;6 ; i++) {
+            tileSet.add(new Tile('T', 1));
+        }
+        </v>
+      </c>
+      <c r="B20" s="19" t="s">
+        <v>95</v>
+      </c>
+      <c r="C20" s="19" t="s">
+        <v>70</v>
+      </c>
+      <c r="D20" s="19" t="s">
+        <v>62</v>
+      </c>
+      <c r="E20" s="19" t="s">
+        <v>42</v>
+      </c>
+      <c r="F20" s="20">
+        <v>6</v>
+      </c>
+      <c r="G20" s="17" t="s">
+        <v>104</v>
+      </c>
+      <c r="H20" s="17" t="s">
+        <v>105</v>
+      </c>
+      <c r="I20" s="18" t="s">
+        <v>106</v>
+      </c>
+      <c r="J20" s="17" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="21" spans="1:10" ht="33" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A21" s="21" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> for (int i = 0; i &lt;5 ; i++) {
+            tileSet.add(new Tile('U', 1));
+        }
+        </v>
+      </c>
+      <c r="B21" s="19" t="s">
+        <v>96</v>
+      </c>
+      <c r="C21" s="19" t="s">
+        <v>70</v>
+      </c>
+      <c r="D21" s="19" t="s">
+        <v>63</v>
+      </c>
+      <c r="E21" s="19" t="s">
+        <v>42</v>
+      </c>
+      <c r="F21" s="20">
+        <v>5</v>
+      </c>
+      <c r="G21" s="17" t="s">
+        <v>104</v>
+      </c>
+      <c r="H21" s="17" t="s">
+        <v>105</v>
+      </c>
+      <c r="I21" s="18" t="s">
+        <v>106</v>
+      </c>
+      <c r="J21" s="17" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="22" spans="1:10" ht="33" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A22" s="21" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> for (int i = 0; i &lt;2 ; i++) {
+            tileSet.add(new Tile('V', 4));
+        }
+        </v>
+      </c>
+      <c r="B22" s="19" t="s">
+        <v>97</v>
+      </c>
+      <c r="C22" s="19" t="s">
+        <v>78</v>
+      </c>
+      <c r="D22" s="19" t="s">
+        <v>64</v>
+      </c>
+      <c r="E22" s="19" t="s">
+        <v>42</v>
+      </c>
+      <c r="F22" s="20">
+        <v>2</v>
+      </c>
+      <c r="G22" s="17" t="s">
+        <v>104</v>
+      </c>
+      <c r="H22" s="17" t="s">
+        <v>105</v>
+      </c>
+      <c r="I22" s="18" t="s">
+        <v>106</v>
+      </c>
+      <c r="J22" s="17" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="23" spans="1:10" ht="33" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A23" s="21" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> for (int i = 0; i &lt;1 ; i++) {
+            tileSet.add(new Tile('W', 4));
+        }
+        </v>
+      </c>
+      <c r="B23" s="19" t="s">
+        <v>98</v>
+      </c>
+      <c r="C23" s="19" t="s">
+        <v>78</v>
+      </c>
+      <c r="D23" s="19" t="s">
+        <v>65</v>
+      </c>
+      <c r="E23" s="19" t="s">
+        <v>42</v>
+      </c>
+      <c r="F23" s="20">
+        <v>1</v>
+      </c>
+      <c r="G23" s="17" t="s">
+        <v>104</v>
+      </c>
+      <c r="H23" s="17" t="s">
+        <v>105</v>
+      </c>
+      <c r="I23" s="18" t="s">
+        <v>106</v>
+      </c>
+      <c r="J23" s="17" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="24" spans="1:10" ht="33" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A24" s="21" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> for (int i = 0; i &lt;1 ; i++) {
+            tileSet.add(new Tile('X', 9));
+        }
+        </v>
+      </c>
+      <c r="B24" s="19" t="s">
+        <v>99</v>
+      </c>
+      <c r="C24" s="19" t="s">
+        <v>83</v>
+      </c>
+      <c r="D24" s="19" t="s">
+        <v>66</v>
+      </c>
+      <c r="E24" s="19" t="s">
+        <v>42</v>
+      </c>
+      <c r="F24" s="20">
+        <v>1</v>
+      </c>
+      <c r="G24" s="17" t="s">
+        <v>104</v>
+      </c>
+      <c r="H24" s="17" t="s">
+        <v>105</v>
+      </c>
+      <c r="I24" s="18" t="s">
+        <v>106</v>
+      </c>
+      <c r="J24" s="17" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="25" spans="1:10" ht="33" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A25" s="21" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> for (int i = 0; i &lt;2 ; i++) {
+            tileSet.add(new Tile('Y', 5));
+        }
+        </v>
+      </c>
+      <c r="B25" s="19" t="s">
+        <v>100</v>
+      </c>
+      <c r="C25" s="19" t="s">
+        <v>101</v>
+      </c>
+      <c r="D25" s="19" t="s">
+        <v>67</v>
+      </c>
+      <c r="E25" s="19" t="s">
+        <v>42</v>
+      </c>
+      <c r="F25" s="20">
+        <v>2</v>
+      </c>
+      <c r="G25" s="17" t="s">
+        <v>104</v>
+      </c>
+      <c r="H25" s="17" t="s">
+        <v>105</v>
+      </c>
+      <c r="I25" s="18" t="s">
+        <v>106</v>
+      </c>
+      <c r="J25" s="17" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="26" spans="1:10" ht="33" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A26" s="21" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> for (int i = 0; i &lt;1 ; i++) {
+            tileSet.add(new Tile('Z', 11));
+        }
+        </v>
+      </c>
+      <c r="B26" s="19" t="s">
+        <v>102</v>
+      </c>
+      <c r="C26" s="19" t="s">
+        <v>103</v>
+      </c>
+      <c r="D26" s="19" t="s">
+        <v>68</v>
+      </c>
+      <c r="E26" s="19" t="s">
+        <v>42</v>
+      </c>
+      <c r="F26" s="20">
+        <v>1</v>
+      </c>
+      <c r="G26" s="17" t="s">
+        <v>104</v>
+      </c>
+      <c r="H26" s="17" t="s">
+        <v>105</v>
+      </c>
+      <c r="I26" s="18" t="s">
+        <v>106</v>
+      </c>
+      <c r="J26" s="17" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="27" spans="1:10" ht="33" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A27" s="21" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> for (int i = 0; i &lt;5 ; i++) {
+            tileSet.add(new Tile('_', 5));
+        }
+        </v>
+      </c>
+      <c r="B27" s="19" t="s">
+        <v>108</v>
+      </c>
+      <c r="C27" s="19">
+        <v>5</v>
+      </c>
+      <c r="D27" s="19" t="s">
+        <v>109</v>
+      </c>
+      <c r="E27" s="19" t="s">
+        <v>42</v>
+      </c>
+      <c r="F27" s="19">
+        <v>5</v>
+      </c>
+      <c r="G27" s="17" t="s">
+        <v>104</v>
+      </c>
+      <c r="H27" s="17" t="s">
+        <v>105</v>
+      </c>
+      <c r="I27" s="18" t="s">
+        <v>106</v>
+      </c>
+      <c r="J27" s="17" t="s">
+        <v>107</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
TileMap() Refactor so now prints key value pairs correctly.
</commit_message>
<xml_diff>
--- a/Ancillary Docs/Default Board Helper File.xlsx
+++ b/Ancillary Docs/Default Board Helper File.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/xeon2035/Library/Mobile Documents/com~apple~CloudDocs/UniWerk/13/Ancillary Docs/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/xeon2035/Library/Mobile Documents/com~apple~CloudDocs/UniWerk/MySkraBBKle/Ancillary Docs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D938FFF1-5DC4-824E-917C-6EE0E81F886E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C147672A-4404-5447-8EE5-767B322AE7EE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="26740" windowHeight="14620" activeTab="3" xr2:uid="{F938695B-E880-FB4D-B508-A292FAB83920}"/>
   </bookViews>
@@ -480,7 +480,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -531,6 +531,13 @@
     <font>
       <sz val="15"/>
       <color rgb="FFFF0000"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="15"/>
+      <color rgb="FF002060"/>
       <name val="Aptos Narrow"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -620,7 +627,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="24">
+  <cellXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -690,6 +697,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -2797,993 +2807,1102 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8E2AA095-8C4D-BA40-8955-A2825FB0D37F}">
-  <dimension ref="A1:J27"/>
+  <dimension ref="A1:K27"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection sqref="A1:A27"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A20" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C32" sqref="C32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="33" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="66.83203125" style="22" customWidth="1"/>
-    <col min="2" max="5" width="10.83203125" style="19"/>
-    <col min="6" max="6" width="13.5" style="19" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="19.33203125" style="22" customWidth="1"/>
-    <col min="8" max="8" width="33.5" style="22" customWidth="1"/>
-    <col min="9" max="9" width="8.33203125" style="22" customWidth="1"/>
-    <col min="10" max="10" width="10.83203125" style="22" customWidth="1"/>
-    <col min="11" max="16384" width="10.83203125" style="22"/>
+    <col min="2" max="2" width="24.83203125" style="22" customWidth="1"/>
+    <col min="3" max="6" width="10.83203125" style="19"/>
+    <col min="7" max="7" width="13.5" style="19" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="19.33203125" style="22" customWidth="1"/>
+    <col min="9" max="9" width="33.5" style="22" customWidth="1"/>
+    <col min="10" max="10" width="8.33203125" style="22" customWidth="1"/>
+    <col min="11" max="11" width="10.83203125" style="22" customWidth="1"/>
+    <col min="12" max="16384" width="10.83203125" style="22"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="33" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:11" ht="33" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="21" t="str">
-        <f t="shared" ref="A1:A27" si="0">G1&amp;F1&amp;H1&amp;B1&amp;"'"&amp;I1&amp;C1&amp;J1</f>
+        <f>H1&amp;G1&amp;I1&amp;C1&amp;"'"&amp;J1&amp;D1&amp;K1</f>
         <v xml:space="preserve"> for (int i = 0; i &lt;8 ; i++) {
             tileSet.add(new Tile('A', 1));
         }
         </v>
       </c>
-      <c r="B1" s="19" t="s">
+      <c r="B1" s="24" t="str">
+        <f>"tileSetMap.put('"&amp;C1&amp;"', "&amp;D1&amp;");"</f>
+        <v>tileSetMap.put('A', 1);</v>
+      </c>
+      <c r="C1" s="19" t="s">
         <v>69</v>
       </c>
-      <c r="C1" s="19" t="s">
+      <c r="D1" s="19" t="s">
         <v>70</v>
       </c>
-      <c r="D1" s="19" t="s">
+      <c r="E1" s="19" t="s">
         <v>43</v>
       </c>
-      <c r="E1" s="19" t="s">
+      <c r="F1" s="19" t="s">
         <v>42</v>
       </c>
-      <c r="F1" s="20">
+      <c r="G1" s="20">
         <v>8</v>
       </c>
-      <c r="G1" s="17" t="s">
+      <c r="H1" s="17" t="s">
         <v>104</v>
       </c>
-      <c r="H1" s="17" t="s">
+      <c r="I1" s="17" t="s">
         <v>105</v>
       </c>
-      <c r="I1" s="18" t="s">
+      <c r="J1" s="18" t="s">
         <v>106</v>
       </c>
-      <c r="J1" s="17" t="s">
+      <c r="K1" s="17" t="s">
         <v>107</v>
       </c>
     </row>
-    <row r="2" spans="1:10" ht="33" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:11" ht="33" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="21" t="str">
-        <f t="shared" si="0"/>
+        <f>H2&amp;G2&amp;I2&amp;C2&amp;"'"&amp;J2&amp;D2&amp;K2</f>
         <v xml:space="preserve"> for (int i = 0; i &lt;2 ; i++) {
             tileSet.add(new Tile('B', 3));
         }
         </v>
       </c>
-      <c r="B2" s="19" t="s">
+      <c r="B2" s="24" t="str">
+        <f t="shared" ref="B2:B27" si="0">"tileSetMap.put('"&amp;C2&amp;"', "&amp;D2&amp;");"</f>
+        <v>tileSetMap.put('B', 3);</v>
+      </c>
+      <c r="C2" s="19" t="s">
         <v>71</v>
       </c>
-      <c r="C2" s="19" t="s">
+      <c r="D2" s="19" t="s">
         <v>72</v>
       </c>
-      <c r="D2" s="19" t="s">
+      <c r="E2" s="19" t="s">
         <v>44</v>
       </c>
-      <c r="E2" s="19" t="s">
+      <c r="F2" s="19" t="s">
         <v>42</v>
       </c>
-      <c r="F2" s="20">
+      <c r="G2" s="20">
         <v>2</v>
       </c>
-      <c r="G2" s="17" t="s">
+      <c r="H2" s="17" t="s">
         <v>104</v>
       </c>
-      <c r="H2" s="17" t="s">
+      <c r="I2" s="17" t="s">
         <v>105</v>
       </c>
-      <c r="I2" s="18" t="s">
+      <c r="J2" s="18" t="s">
         <v>106</v>
       </c>
-      <c r="J2" s="17" t="s">
+      <c r="K2" s="17" t="s">
         <v>107</v>
       </c>
     </row>
-    <row r="3" spans="1:10" ht="33" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:11" ht="33" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="21" t="str">
-        <f t="shared" si="0"/>
+        <f>H3&amp;G3&amp;I3&amp;C3&amp;"'"&amp;J3&amp;D3&amp;K3</f>
         <v xml:space="preserve"> for (int i = 0; i &lt;2 ; i++) {
             tileSet.add(new Tile('C', 3));
         }
         </v>
       </c>
-      <c r="B3" s="19" t="s">
+      <c r="B3" s="24" t="str">
+        <f t="shared" si="0"/>
+        <v>tileSetMap.put('C', 3);</v>
+      </c>
+      <c r="C3" s="19" t="s">
         <v>73</v>
       </c>
-      <c r="C3" s="19" t="s">
+      <c r="D3" s="19" t="s">
         <v>72</v>
       </c>
-      <c r="D3" s="19" t="s">
+      <c r="E3" s="19" t="s">
         <v>45</v>
       </c>
-      <c r="E3" s="19" t="s">
+      <c r="F3" s="19" t="s">
         <v>42</v>
       </c>
-      <c r="F3" s="20">
+      <c r="G3" s="20">
         <v>2</v>
       </c>
-      <c r="G3" s="17" t="s">
+      <c r="H3" s="17" t="s">
         <v>104</v>
       </c>
-      <c r="H3" s="17" t="s">
+      <c r="I3" s="17" t="s">
         <v>105</v>
       </c>
-      <c r="I3" s="18" t="s">
+      <c r="J3" s="18" t="s">
         <v>106</v>
       </c>
-      <c r="J3" s="17" t="s">
+      <c r="K3" s="17" t="s">
         <v>107</v>
       </c>
     </row>
-    <row r="4" spans="1:10" ht="33" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:11" ht="33" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="21" t="str">
-        <f t="shared" si="0"/>
+        <f>H4&amp;G4&amp;I4&amp;C4&amp;"'"&amp;J4&amp;D4&amp;K4</f>
         <v xml:space="preserve"> for (int i = 0; i &lt;4 ; i++) {
             tileSet.add(new Tile('D', 2));
         }
         </v>
       </c>
-      <c r="B4" s="19" t="s">
+      <c r="B4" s="24" t="str">
+        <f t="shared" si="0"/>
+        <v>tileSetMap.put('D', 2);</v>
+      </c>
+      <c r="C4" s="19" t="s">
         <v>74</v>
       </c>
-      <c r="C4" s="19" t="s">
+      <c r="D4" s="19" t="s">
         <v>75</v>
       </c>
-      <c r="D4" s="19" t="s">
+      <c r="E4" s="19" t="s">
         <v>46</v>
       </c>
-      <c r="E4" s="19" t="s">
+      <c r="F4" s="19" t="s">
         <v>42</v>
       </c>
-      <c r="F4" s="20">
+      <c r="G4" s="20">
         <v>4</v>
       </c>
-      <c r="G4" s="17" t="s">
+      <c r="H4" s="17" t="s">
         <v>104</v>
       </c>
-      <c r="H4" s="17" t="s">
+      <c r="I4" s="17" t="s">
         <v>105</v>
       </c>
-      <c r="I4" s="18" t="s">
+      <c r="J4" s="18" t="s">
         <v>106</v>
       </c>
-      <c r="J4" s="17" t="s">
+      <c r="K4" s="17" t="s">
         <v>107</v>
       </c>
     </row>
-    <row r="5" spans="1:10" ht="33" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:11" ht="33" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="21" t="str">
-        <f t="shared" si="0"/>
+        <f>H5&amp;G5&amp;I5&amp;C5&amp;"'"&amp;J5&amp;D5&amp;K5</f>
         <v xml:space="preserve"> for (int i = 0; i &lt;10 ; i++) {
             tileSet.add(new Tile('E', 1));
         }
         </v>
       </c>
-      <c r="B5" s="19" t="s">
+      <c r="B5" s="24" t="str">
+        <f t="shared" si="0"/>
+        <v>tileSetMap.put('E', 1);</v>
+      </c>
+      <c r="C5" s="19" t="s">
         <v>76</v>
       </c>
-      <c r="C5" s="19" t="s">
+      <c r="D5" s="19" t="s">
         <v>70</v>
       </c>
-      <c r="D5" s="19" t="s">
+      <c r="E5" s="19" t="s">
         <v>47</v>
       </c>
-      <c r="E5" s="19" t="s">
+      <c r="F5" s="19" t="s">
         <v>42</v>
       </c>
-      <c r="F5" s="20">
+      <c r="G5" s="20">
         <v>10</v>
       </c>
-      <c r="G5" s="17" t="s">
+      <c r="H5" s="17" t="s">
         <v>104</v>
       </c>
-      <c r="H5" s="17" t="s">
+      <c r="I5" s="17" t="s">
         <v>105</v>
       </c>
-      <c r="I5" s="18" t="s">
+      <c r="J5" s="18" t="s">
         <v>106</v>
       </c>
-      <c r="J5" s="17" t="s">
+      <c r="K5" s="17" t="s">
         <v>107</v>
       </c>
     </row>
-    <row r="6" spans="1:10" ht="33" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:11" ht="33" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="21" t="str">
-        <f t="shared" si="0"/>
+        <f>H6&amp;G6&amp;I6&amp;C6&amp;"'"&amp;J6&amp;D6&amp;K6</f>
         <v xml:space="preserve"> for (int i = 0; i &lt;3 ; i++) {
             tileSet.add(new Tile('F', 4));
         }
         </v>
       </c>
-      <c r="B6" s="19" t="s">
+      <c r="B6" s="24" t="str">
+        <f t="shared" si="0"/>
+        <v>tileSetMap.put('F', 4);</v>
+      </c>
+      <c r="C6" s="19" t="s">
         <v>77</v>
       </c>
-      <c r="C6" s="19" t="s">
+      <c r="D6" s="19" t="s">
         <v>78</v>
       </c>
-      <c r="D6" s="19" t="s">
+      <c r="E6" s="19" t="s">
         <v>48</v>
       </c>
-      <c r="E6" s="19" t="s">
+      <c r="F6" s="19" t="s">
         <v>42</v>
       </c>
-      <c r="F6" s="20">
+      <c r="G6" s="20">
         <v>3</v>
       </c>
-      <c r="G6" s="17" t="s">
+      <c r="H6" s="17" t="s">
         <v>104</v>
       </c>
-      <c r="H6" s="17" t="s">
+      <c r="I6" s="17" t="s">
         <v>105</v>
       </c>
-      <c r="I6" s="18" t="s">
+      <c r="J6" s="18" t="s">
         <v>106</v>
       </c>
-      <c r="J6" s="17" t="s">
+      <c r="K6" s="17" t="s">
         <v>107</v>
       </c>
     </row>
-    <row r="7" spans="1:10" ht="33" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:11" ht="33" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="21" t="str">
-        <f t="shared" si="0"/>
+        <f>H7&amp;G7&amp;I7&amp;C7&amp;"'"&amp;J7&amp;D7&amp;K7</f>
         <v xml:space="preserve"> for (int i = 0; i &lt;4 ; i++) {
             tileSet.add(new Tile('G', 2));
         }
         </v>
       </c>
-      <c r="B7" s="19" t="s">
+      <c r="B7" s="24" t="str">
+        <f t="shared" si="0"/>
+        <v>tileSetMap.put('G', 2);</v>
+      </c>
+      <c r="C7" s="19" t="s">
         <v>79</v>
       </c>
-      <c r="C7" s="19" t="s">
+      <c r="D7" s="19" t="s">
         <v>75</v>
       </c>
-      <c r="D7" s="19" t="s">
+      <c r="E7" s="19" t="s">
         <v>49</v>
       </c>
-      <c r="E7" s="19" t="s">
+      <c r="F7" s="19" t="s">
         <v>42</v>
       </c>
-      <c r="F7" s="20">
+      <c r="G7" s="20">
         <v>4</v>
       </c>
-      <c r="G7" s="17" t="s">
+      <c r="H7" s="17" t="s">
         <v>104</v>
       </c>
-      <c r="H7" s="17" t="s">
+      <c r="I7" s="17" t="s">
         <v>105</v>
       </c>
-      <c r="I7" s="18" t="s">
+      <c r="J7" s="18" t="s">
         <v>106</v>
       </c>
-      <c r="J7" s="17" t="s">
+      <c r="K7" s="17" t="s">
         <v>107</v>
       </c>
     </row>
-    <row r="8" spans="1:10" ht="33" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:11" ht="33" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="21" t="str">
-        <f t="shared" si="0"/>
+        <f>H8&amp;G8&amp;I8&amp;C8&amp;"'"&amp;J8&amp;D8&amp;K8</f>
         <v xml:space="preserve"> for (int i = 0; i &lt;3 ; i++) {
             tileSet.add(new Tile('H', 4));
         }
         </v>
       </c>
-      <c r="B8" s="19" t="s">
+      <c r="B8" s="24" t="str">
+        <f t="shared" si="0"/>
+        <v>tileSetMap.put('H', 4);</v>
+      </c>
+      <c r="C8" s="19" t="s">
         <v>80</v>
       </c>
-      <c r="C8" s="19" t="s">
+      <c r="D8" s="19" t="s">
         <v>78</v>
       </c>
-      <c r="D8" s="19" t="s">
+      <c r="E8" s="19" t="s">
         <v>50</v>
       </c>
-      <c r="E8" s="19" t="s">
+      <c r="F8" s="19" t="s">
         <v>42</v>
       </c>
-      <c r="F8" s="20">
+      <c r="G8" s="20">
         <v>3</v>
       </c>
-      <c r="G8" s="17" t="s">
+      <c r="H8" s="17" t="s">
         <v>104</v>
       </c>
-      <c r="H8" s="17" t="s">
+      <c r="I8" s="17" t="s">
         <v>105</v>
       </c>
-      <c r="I8" s="18" t="s">
+      <c r="J8" s="18" t="s">
         <v>106</v>
       </c>
-      <c r="J8" s="17" t="s">
+      <c r="K8" s="17" t="s">
         <v>107</v>
       </c>
     </row>
-    <row r="9" spans="1:10" ht="33" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:11" ht="33" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="21" t="str">
-        <f t="shared" si="0"/>
+        <f>H9&amp;G9&amp;I9&amp;C9&amp;"'"&amp;J9&amp;D9&amp;K9</f>
         <v xml:space="preserve"> for (int i = 0; i &lt;8 ; i++) {
             tileSet.add(new Tile('I', 1));
         }
         </v>
       </c>
-      <c r="B9" s="19" t="s">
+      <c r="B9" s="24" t="str">
+        <f t="shared" si="0"/>
+        <v>tileSetMap.put('I', 1);</v>
+      </c>
+      <c r="C9" s="19" t="s">
         <v>81</v>
       </c>
-      <c r="C9" s="19" t="s">
+      <c r="D9" s="19" t="s">
         <v>70</v>
       </c>
-      <c r="D9" s="19" t="s">
+      <c r="E9" s="19" t="s">
         <v>51</v>
       </c>
-      <c r="E9" s="19" t="s">
+      <c r="F9" s="19" t="s">
         <v>42</v>
       </c>
-      <c r="F9" s="20">
+      <c r="G9" s="20">
         <v>8</v>
       </c>
-      <c r="G9" s="17" t="s">
+      <c r="H9" s="17" t="s">
         <v>104</v>
       </c>
-      <c r="H9" s="17" t="s">
+      <c r="I9" s="17" t="s">
         <v>105</v>
       </c>
-      <c r="I9" s="18" t="s">
+      <c r="J9" s="18" t="s">
         <v>106</v>
       </c>
-      <c r="J9" s="17" t="s">
+      <c r="K9" s="17" t="s">
         <v>107</v>
       </c>
     </row>
-    <row r="10" spans="1:10" ht="33" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:11" ht="33" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="21" t="str">
-        <f t="shared" si="0"/>
+        <f>H10&amp;G10&amp;I10&amp;C10&amp;"'"&amp;J10&amp;D10&amp;K10</f>
         <v xml:space="preserve"> for (int i = 0; i &lt;1 ; i++) {
             tileSet.add(new Tile('J', 9));
         }
         </v>
       </c>
-      <c r="B10" s="19" t="s">
+      <c r="B10" s="24" t="str">
+        <f t="shared" si="0"/>
+        <v>tileSetMap.put('J', 9);</v>
+      </c>
+      <c r="C10" s="19" t="s">
         <v>82</v>
       </c>
-      <c r="C10" s="19" t="s">
+      <c r="D10" s="19" t="s">
         <v>83</v>
       </c>
-      <c r="D10" s="19" t="s">
+      <c r="E10" s="19" t="s">
         <v>52</v>
       </c>
-      <c r="E10" s="19" t="s">
+      <c r="F10" s="19" t="s">
         <v>42</v>
       </c>
-      <c r="F10" s="20">
+      <c r="G10" s="20">
         <v>1</v>
       </c>
-      <c r="G10" s="17" t="s">
+      <c r="H10" s="17" t="s">
         <v>104</v>
       </c>
-      <c r="H10" s="17" t="s">
+      <c r="I10" s="17" t="s">
         <v>105</v>
       </c>
-      <c r="I10" s="18" t="s">
+      <c r="J10" s="18" t="s">
         <v>106</v>
       </c>
-      <c r="J10" s="17" t="s">
+      <c r="K10" s="17" t="s">
         <v>107</v>
       </c>
     </row>
-    <row r="11" spans="1:10" ht="33" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:11" ht="33" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="21" t="str">
-        <f t="shared" si="0"/>
+        <f>H11&amp;G11&amp;I11&amp;C11&amp;"'"&amp;J11&amp;D11&amp;K11</f>
         <v xml:space="preserve"> for (int i = 0; i &lt;1 ; i++) {
             tileSet.add(new Tile('K', 6));
         }
         </v>
       </c>
-      <c r="B11" s="19" t="s">
+      <c r="B11" s="24" t="str">
+        <f t="shared" si="0"/>
+        <v>tileSetMap.put('K', 6);</v>
+      </c>
+      <c r="C11" s="19" t="s">
         <v>84</v>
       </c>
-      <c r="C11" s="19" t="s">
+      <c r="D11" s="19" t="s">
         <v>85</v>
       </c>
-      <c r="D11" s="19" t="s">
+      <c r="E11" s="19" t="s">
         <v>53</v>
       </c>
-      <c r="E11" s="19" t="s">
+      <c r="F11" s="19" t="s">
         <v>42</v>
       </c>
-      <c r="F11" s="20">
+      <c r="G11" s="20">
         <v>1</v>
       </c>
-      <c r="G11" s="17" t="s">
+      <c r="H11" s="17" t="s">
         <v>104</v>
       </c>
-      <c r="H11" s="17" t="s">
+      <c r="I11" s="17" t="s">
         <v>105</v>
       </c>
-      <c r="I11" s="18" t="s">
+      <c r="J11" s="18" t="s">
         <v>106</v>
       </c>
-      <c r="J11" s="17" t="s">
+      <c r="K11" s="17" t="s">
         <v>107</v>
       </c>
     </row>
-    <row r="12" spans="1:10" ht="33" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:11" ht="33" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="21" t="str">
-        <f t="shared" si="0"/>
+        <f>H12&amp;G12&amp;I12&amp;C12&amp;"'"&amp;J12&amp;D12&amp;K12</f>
         <v xml:space="preserve"> for (int i = 0; i &lt;4 ; i++) {
             tileSet.add(new Tile('L', 1));
         }
         </v>
       </c>
-      <c r="B12" s="19" t="s">
+      <c r="B12" s="24" t="str">
+        <f t="shared" si="0"/>
+        <v>tileSetMap.put('L', 1);</v>
+      </c>
+      <c r="C12" s="19" t="s">
         <v>86</v>
       </c>
-      <c r="C12" s="19" t="s">
+      <c r="D12" s="19" t="s">
         <v>70</v>
       </c>
-      <c r="D12" s="19" t="s">
+      <c r="E12" s="19" t="s">
         <v>54</v>
       </c>
-      <c r="E12" s="19" t="s">
+      <c r="F12" s="19" t="s">
         <v>42</v>
       </c>
-      <c r="F12" s="20">
+      <c r="G12" s="20">
         <v>4</v>
       </c>
-      <c r="G12" s="17" t="s">
+      <c r="H12" s="17" t="s">
         <v>104</v>
       </c>
-      <c r="H12" s="17" t="s">
+      <c r="I12" s="17" t="s">
         <v>105</v>
       </c>
-      <c r="I12" s="18" t="s">
+      <c r="J12" s="18" t="s">
         <v>106</v>
       </c>
-      <c r="J12" s="17" t="s">
+      <c r="K12" s="17" t="s">
         <v>107</v>
       </c>
     </row>
-    <row r="13" spans="1:10" ht="33" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:11" ht="33" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="21" t="str">
-        <f t="shared" si="0"/>
+        <f>H13&amp;G13&amp;I13&amp;C13&amp;"'"&amp;J13&amp;D13&amp;K13</f>
         <v xml:space="preserve"> for (int i = 0; i &lt;2 ; i++) {
             tileSet.add(new Tile('M', 3));
         }
         </v>
       </c>
-      <c r="B13" s="19" t="s">
+      <c r="B13" s="24" t="str">
+        <f t="shared" si="0"/>
+        <v>tileSetMap.put('M', 3);</v>
+      </c>
+      <c r="C13" s="19" t="s">
         <v>87</v>
       </c>
-      <c r="C13" s="19" t="s">
+      <c r="D13" s="19" t="s">
         <v>72</v>
       </c>
-      <c r="D13" s="19" t="s">
+      <c r="E13" s="19" t="s">
         <v>55</v>
       </c>
-      <c r="E13" s="19" t="s">
+      <c r="F13" s="19" t="s">
         <v>42</v>
       </c>
-      <c r="F13" s="20">
+      <c r="G13" s="20">
         <v>2</v>
       </c>
-      <c r="G13" s="17" t="s">
+      <c r="H13" s="17" t="s">
         <v>104</v>
       </c>
-      <c r="H13" s="17" t="s">
+      <c r="I13" s="17" t="s">
         <v>105</v>
       </c>
-      <c r="I13" s="18" t="s">
+      <c r="J13" s="18" t="s">
         <v>106</v>
       </c>
-      <c r="J13" s="17" t="s">
+      <c r="K13" s="17" t="s">
         <v>107</v>
       </c>
     </row>
-    <row r="14" spans="1:10" ht="33" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:11" ht="33" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="21" t="str">
-        <f t="shared" si="0"/>
+        <f>H14&amp;G14&amp;I14&amp;C14&amp;"'"&amp;J14&amp;D14&amp;K14</f>
         <v xml:space="preserve"> for (int i = 0; i &lt;7 ; i++) {
             tileSet.add(new Tile('N', 1));
         }
         </v>
       </c>
-      <c r="B14" s="19" t="s">
+      <c r="B14" s="24" t="str">
+        <f t="shared" si="0"/>
+        <v>tileSetMap.put('N', 1);</v>
+      </c>
+      <c r="C14" s="19" t="s">
         <v>88</v>
       </c>
-      <c r="C14" s="19" t="s">
+      <c r="D14" s="19" t="s">
         <v>70</v>
       </c>
-      <c r="D14" s="19" t="s">
+      <c r="E14" s="19" t="s">
         <v>56</v>
       </c>
-      <c r="E14" s="19" t="s">
+      <c r="F14" s="19" t="s">
         <v>42</v>
       </c>
-      <c r="F14" s="20">
+      <c r="G14" s="20">
         <v>7</v>
       </c>
-      <c r="G14" s="17" t="s">
+      <c r="H14" s="17" t="s">
         <v>104</v>
       </c>
-      <c r="H14" s="17" t="s">
+      <c r="I14" s="17" t="s">
         <v>105</v>
       </c>
-      <c r="I14" s="18" t="s">
+      <c r="J14" s="18" t="s">
         <v>106</v>
       </c>
-      <c r="J14" s="17" t="s">
+      <c r="K14" s="17" t="s">
         <v>107</v>
       </c>
     </row>
-    <row r="15" spans="1:10" ht="33" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:11" ht="33" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="21" t="str">
-        <f t="shared" si="0"/>
+        <f>H15&amp;G15&amp;I15&amp;C15&amp;"'"&amp;J15&amp;D15&amp;K15</f>
         <v xml:space="preserve"> for (int i = 0; i &lt;7 ; i++) {
             tileSet.add(new Tile('O', 1));
         }
         </v>
       </c>
-      <c r="B15" s="19" t="s">
+      <c r="B15" s="24" t="str">
+        <f t="shared" si="0"/>
+        <v>tileSetMap.put('O', 1);</v>
+      </c>
+      <c r="C15" s="19" t="s">
         <v>89</v>
       </c>
-      <c r="C15" s="19" t="s">
+      <c r="D15" s="19" t="s">
         <v>70</v>
       </c>
-      <c r="D15" s="19" t="s">
+      <c r="E15" s="19" t="s">
         <v>57</v>
       </c>
-      <c r="E15" s="19" t="s">
+      <c r="F15" s="19" t="s">
         <v>42</v>
       </c>
-      <c r="F15" s="20">
+      <c r="G15" s="20">
         <v>7</v>
       </c>
-      <c r="G15" s="17" t="s">
+      <c r="H15" s="17" t="s">
         <v>104</v>
       </c>
-      <c r="H15" s="17" t="s">
+      <c r="I15" s="17" t="s">
         <v>105</v>
       </c>
-      <c r="I15" s="18" t="s">
+      <c r="J15" s="18" t="s">
         <v>106</v>
       </c>
-      <c r="J15" s="17" t="s">
+      <c r="K15" s="17" t="s">
         <v>107</v>
       </c>
     </row>
-    <row r="16" spans="1:10" ht="33" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:11" ht="33" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="21" t="str">
-        <f t="shared" si="0"/>
+        <f>H16&amp;G16&amp;I16&amp;C16&amp;"'"&amp;J16&amp;D16&amp;K16</f>
         <v xml:space="preserve"> for (int i = 0; i &lt;2 ; i++) {
             tileSet.add(new Tile('P', 3));
         }
         </v>
       </c>
-      <c r="B16" s="19" t="s">
+      <c r="B16" s="24" t="str">
+        <f t="shared" si="0"/>
+        <v>tileSetMap.put('P', 3);</v>
+      </c>
+      <c r="C16" s="19" t="s">
         <v>90</v>
       </c>
-      <c r="C16" s="19" t="s">
+      <c r="D16" s="19" t="s">
         <v>72</v>
       </c>
-      <c r="D16" s="19" t="s">
+      <c r="E16" s="19" t="s">
         <v>58</v>
       </c>
-      <c r="E16" s="19" t="s">
+      <c r="F16" s="19" t="s">
         <v>42</v>
       </c>
-      <c r="F16" s="20">
+      <c r="G16" s="20">
         <v>2</v>
       </c>
-      <c r="G16" s="17" t="s">
+      <c r="H16" s="17" t="s">
         <v>104</v>
       </c>
-      <c r="H16" s="17" t="s">
+      <c r="I16" s="17" t="s">
         <v>105</v>
       </c>
-      <c r="I16" s="18" t="s">
+      <c r="J16" s="18" t="s">
         <v>106</v>
       </c>
-      <c r="J16" s="17" t="s">
+      <c r="K16" s="17" t="s">
         <v>107</v>
       </c>
     </row>
-    <row r="17" spans="1:10" ht="33" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:11" ht="33" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" s="21" t="str">
-        <f t="shared" si="0"/>
+        <f>H17&amp;G17&amp;I17&amp;C17&amp;"'"&amp;J17&amp;D17&amp;K17</f>
         <v xml:space="preserve"> for (int i = 0; i &lt;1 ; i++) {
             tileSet.add(new Tile('Q', 12));
         }
         </v>
       </c>
-      <c r="B17" s="19" t="s">
+      <c r="B17" s="24" t="str">
+        <f t="shared" si="0"/>
+        <v>tileSetMap.put('Q', 12);</v>
+      </c>
+      <c r="C17" s="19" t="s">
         <v>91</v>
       </c>
-      <c r="C17" s="19" t="s">
+      <c r="D17" s="19" t="s">
         <v>92</v>
       </c>
-      <c r="D17" s="19" t="s">
+      <c r="E17" s="19" t="s">
         <v>59</v>
       </c>
-      <c r="E17" s="19" t="s">
+      <c r="F17" s="19" t="s">
         <v>42</v>
       </c>
-      <c r="F17" s="20">
+      <c r="G17" s="20">
         <v>1</v>
       </c>
-      <c r="G17" s="17" t="s">
+      <c r="H17" s="17" t="s">
         <v>104</v>
       </c>
-      <c r="H17" s="17" t="s">
+      <c r="I17" s="17" t="s">
         <v>105</v>
       </c>
-      <c r="I17" s="18" t="s">
+      <c r="J17" s="18" t="s">
         <v>106</v>
       </c>
-      <c r="J17" s="17" t="s">
+      <c r="K17" s="17" t="s">
         <v>107</v>
       </c>
     </row>
-    <row r="18" spans="1:10" ht="33" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:11" ht="33" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" s="21" t="str">
-        <f t="shared" si="0"/>
+        <f>H18&amp;G18&amp;I18&amp;C18&amp;"'"&amp;J18&amp;D18&amp;K18</f>
         <v xml:space="preserve"> for (int i = 0; i &lt;6 ; i++) {
             tileSet.add(new Tile('R', 1));
         }
         </v>
       </c>
-      <c r="B18" s="19" t="s">
+      <c r="B18" s="24" t="str">
+        <f t="shared" si="0"/>
+        <v>tileSetMap.put('R', 1);</v>
+      </c>
+      <c r="C18" s="19" t="s">
         <v>93</v>
       </c>
-      <c r="C18" s="19" t="s">
+      <c r="D18" s="19" t="s">
         <v>70</v>
       </c>
-      <c r="D18" s="19" t="s">
+      <c r="E18" s="19" t="s">
         <v>60</v>
       </c>
-      <c r="E18" s="19" t="s">
+      <c r="F18" s="19" t="s">
         <v>42</v>
       </c>
-      <c r="F18" s="20">
+      <c r="G18" s="20">
         <v>6</v>
       </c>
-      <c r="G18" s="17" t="s">
+      <c r="H18" s="17" t="s">
         <v>104</v>
       </c>
-      <c r="H18" s="17" t="s">
+      <c r="I18" s="17" t="s">
         <v>105</v>
       </c>
-      <c r="I18" s="18" t="s">
+      <c r="J18" s="18" t="s">
         <v>106</v>
       </c>
-      <c r="J18" s="17" t="s">
+      <c r="K18" s="17" t="s">
         <v>107</v>
       </c>
     </row>
-    <row r="19" spans="1:10" ht="33" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:11" ht="33" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A19" s="21" t="str">
-        <f t="shared" si="0"/>
+        <f>H19&amp;G19&amp;I19&amp;C19&amp;"'"&amp;J19&amp;D19&amp;K19</f>
         <v xml:space="preserve"> for (int i = 0; i &lt;4 ; i++) {
             tileSet.add(new Tile('S', 1));
         }
         </v>
       </c>
-      <c r="B19" s="19" t="s">
+      <c r="B19" s="24" t="str">
+        <f t="shared" si="0"/>
+        <v>tileSetMap.put('S', 1);</v>
+      </c>
+      <c r="C19" s="19" t="s">
         <v>94</v>
       </c>
-      <c r="C19" s="19" t="s">
+      <c r="D19" s="19" t="s">
         <v>70</v>
       </c>
-      <c r="D19" s="19" t="s">
+      <c r="E19" s="19" t="s">
         <v>61</v>
       </c>
-      <c r="E19" s="19" t="s">
+      <c r="F19" s="19" t="s">
         <v>42</v>
       </c>
-      <c r="F19" s="20">
+      <c r="G19" s="20">
         <v>4</v>
       </c>
-      <c r="G19" s="17" t="s">
+      <c r="H19" s="17" t="s">
         <v>104</v>
       </c>
-      <c r="H19" s="17" t="s">
+      <c r="I19" s="17" t="s">
         <v>105</v>
       </c>
-      <c r="I19" s="18" t="s">
+      <c r="J19" s="18" t="s">
         <v>106</v>
       </c>
-      <c r="J19" s="17" t="s">
+      <c r="K19" s="17" t="s">
         <v>107</v>
       </c>
     </row>
-    <row r="20" spans="1:10" ht="33" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:11" ht="33" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A20" s="21" t="str">
-        <f t="shared" si="0"/>
+        <f>H20&amp;G20&amp;I20&amp;C20&amp;"'"&amp;J20&amp;D20&amp;K20</f>
         <v xml:space="preserve"> for (int i = 0; i &lt;6 ; i++) {
             tileSet.add(new Tile('T', 1));
         }
         </v>
       </c>
-      <c r="B20" s="19" t="s">
+      <c r="B20" s="24" t="str">
+        <f t="shared" si="0"/>
+        <v>tileSetMap.put('T', 1);</v>
+      </c>
+      <c r="C20" s="19" t="s">
         <v>95</v>
       </c>
-      <c r="C20" s="19" t="s">
+      <c r="D20" s="19" t="s">
         <v>70</v>
       </c>
-      <c r="D20" s="19" t="s">
+      <c r="E20" s="19" t="s">
         <v>62</v>
       </c>
-      <c r="E20" s="19" t="s">
+      <c r="F20" s="19" t="s">
         <v>42</v>
       </c>
-      <c r="F20" s="20">
+      <c r="G20" s="20">
         <v>6</v>
       </c>
-      <c r="G20" s="17" t="s">
+      <c r="H20" s="17" t="s">
         <v>104</v>
       </c>
-      <c r="H20" s="17" t="s">
+      <c r="I20" s="17" t="s">
         <v>105</v>
       </c>
-      <c r="I20" s="18" t="s">
+      <c r="J20" s="18" t="s">
         <v>106</v>
       </c>
-      <c r="J20" s="17" t="s">
+      <c r="K20" s="17" t="s">
         <v>107</v>
       </c>
     </row>
-    <row r="21" spans="1:10" ht="33" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:11" ht="33" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A21" s="21" t="str">
-        <f t="shared" si="0"/>
+        <f>H21&amp;G21&amp;I21&amp;C21&amp;"'"&amp;J21&amp;D21&amp;K21</f>
         <v xml:space="preserve"> for (int i = 0; i &lt;5 ; i++) {
             tileSet.add(new Tile('U', 1));
         }
         </v>
       </c>
-      <c r="B21" s="19" t="s">
+      <c r="B21" s="24" t="str">
+        <f t="shared" si="0"/>
+        <v>tileSetMap.put('U', 1);</v>
+      </c>
+      <c r="C21" s="19" t="s">
         <v>96</v>
       </c>
-      <c r="C21" s="19" t="s">
+      <c r="D21" s="19" t="s">
         <v>70</v>
       </c>
-      <c r="D21" s="19" t="s">
+      <c r="E21" s="19" t="s">
         <v>63</v>
       </c>
-      <c r="E21" s="19" t="s">
+      <c r="F21" s="19" t="s">
         <v>42</v>
       </c>
-      <c r="F21" s="20">
+      <c r="G21" s="20">
         <v>5</v>
       </c>
-      <c r="G21" s="17" t="s">
+      <c r="H21" s="17" t="s">
         <v>104</v>
       </c>
-      <c r="H21" s="17" t="s">
+      <c r="I21" s="17" t="s">
         <v>105</v>
       </c>
-      <c r="I21" s="18" t="s">
+      <c r="J21" s="18" t="s">
         <v>106</v>
       </c>
-      <c r="J21" s="17" t="s">
+      <c r="K21" s="17" t="s">
         <v>107</v>
       </c>
     </row>
-    <row r="22" spans="1:10" ht="33" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:11" ht="33" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A22" s="21" t="str">
-        <f t="shared" si="0"/>
+        <f>H22&amp;G22&amp;I22&amp;C22&amp;"'"&amp;J22&amp;D22&amp;K22</f>
         <v xml:space="preserve"> for (int i = 0; i &lt;2 ; i++) {
             tileSet.add(new Tile('V', 4));
         }
         </v>
       </c>
-      <c r="B22" s="19" t="s">
+      <c r="B22" s="24" t="str">
+        <f t="shared" si="0"/>
+        <v>tileSetMap.put('V', 4);</v>
+      </c>
+      <c r="C22" s="19" t="s">
         <v>97</v>
       </c>
-      <c r="C22" s="19" t="s">
+      <c r="D22" s="19" t="s">
         <v>78</v>
       </c>
-      <c r="D22" s="19" t="s">
+      <c r="E22" s="19" t="s">
         <v>64</v>
       </c>
-      <c r="E22" s="19" t="s">
+      <c r="F22" s="19" t="s">
         <v>42</v>
       </c>
-      <c r="F22" s="20">
+      <c r="G22" s="20">
         <v>2</v>
       </c>
-      <c r="G22" s="17" t="s">
+      <c r="H22" s="17" t="s">
         <v>104</v>
       </c>
-      <c r="H22" s="17" t="s">
+      <c r="I22" s="17" t="s">
         <v>105</v>
       </c>
-      <c r="I22" s="18" t="s">
+      <c r="J22" s="18" t="s">
         <v>106</v>
       </c>
-      <c r="J22" s="17" t="s">
+      <c r="K22" s="17" t="s">
         <v>107</v>
       </c>
     </row>
-    <row r="23" spans="1:10" ht="33" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:11" ht="33" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A23" s="21" t="str">
-        <f t="shared" si="0"/>
+        <f>H23&amp;G23&amp;I23&amp;C23&amp;"'"&amp;J23&amp;D23&amp;K23</f>
         <v xml:space="preserve"> for (int i = 0; i &lt;1 ; i++) {
             tileSet.add(new Tile('W', 4));
         }
         </v>
       </c>
-      <c r="B23" s="19" t="s">
+      <c r="B23" s="24" t="str">
+        <f t="shared" si="0"/>
+        <v>tileSetMap.put('W', 4);</v>
+      </c>
+      <c r="C23" s="19" t="s">
         <v>98</v>
       </c>
-      <c r="C23" s="19" t="s">
+      <c r="D23" s="19" t="s">
         <v>78</v>
       </c>
-      <c r="D23" s="19" t="s">
+      <c r="E23" s="19" t="s">
         <v>65</v>
       </c>
-      <c r="E23" s="19" t="s">
+      <c r="F23" s="19" t="s">
         <v>42</v>
       </c>
-      <c r="F23" s="20">
+      <c r="G23" s="20">
         <v>1</v>
       </c>
-      <c r="G23" s="17" t="s">
+      <c r="H23" s="17" t="s">
         <v>104</v>
       </c>
-      <c r="H23" s="17" t="s">
+      <c r="I23" s="17" t="s">
         <v>105</v>
       </c>
-      <c r="I23" s="18" t="s">
+      <c r="J23" s="18" t="s">
         <v>106</v>
       </c>
-      <c r="J23" s="17" t="s">
+      <c r="K23" s="17" t="s">
         <v>107</v>
       </c>
     </row>
-    <row r="24" spans="1:10" ht="33" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:11" ht="33" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A24" s="21" t="str">
-        <f t="shared" si="0"/>
+        <f>H24&amp;G24&amp;I24&amp;C24&amp;"'"&amp;J24&amp;D24&amp;K24</f>
         <v xml:space="preserve"> for (int i = 0; i &lt;1 ; i++) {
             tileSet.add(new Tile('X', 9));
         }
         </v>
       </c>
-      <c r="B24" s="19" t="s">
+      <c r="B24" s="24" t="str">
+        <f t="shared" si="0"/>
+        <v>tileSetMap.put('X', 9);</v>
+      </c>
+      <c r="C24" s="19" t="s">
         <v>99</v>
       </c>
-      <c r="C24" s="19" t="s">
+      <c r="D24" s="19" t="s">
         <v>83</v>
       </c>
-      <c r="D24" s="19" t="s">
+      <c r="E24" s="19" t="s">
         <v>66</v>
       </c>
-      <c r="E24" s="19" t="s">
+      <c r="F24" s="19" t="s">
         <v>42</v>
       </c>
-      <c r="F24" s="20">
+      <c r="G24" s="20">
         <v>1</v>
       </c>
-      <c r="G24" s="17" t="s">
+      <c r="H24" s="17" t="s">
         <v>104</v>
       </c>
-      <c r="H24" s="17" t="s">
+      <c r="I24" s="17" t="s">
         <v>105</v>
       </c>
-      <c r="I24" s="18" t="s">
+      <c r="J24" s="18" t="s">
         <v>106</v>
       </c>
-      <c r="J24" s="17" t="s">
+      <c r="K24" s="17" t="s">
         <v>107</v>
       </c>
     </row>
-    <row r="25" spans="1:10" ht="33" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:11" ht="33" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A25" s="21" t="str">
-        <f t="shared" si="0"/>
+        <f>H25&amp;G25&amp;I25&amp;C25&amp;"'"&amp;J25&amp;D25&amp;K25</f>
         <v xml:space="preserve"> for (int i = 0; i &lt;2 ; i++) {
             tileSet.add(new Tile('Y', 5));
         }
         </v>
       </c>
-      <c r="B25" s="19" t="s">
+      <c r="B25" s="24" t="str">
+        <f t="shared" si="0"/>
+        <v>tileSetMap.put('Y', 5);</v>
+      </c>
+      <c r="C25" s="19" t="s">
         <v>100</v>
       </c>
-      <c r="C25" s="19" t="s">
+      <c r="D25" s="19" t="s">
         <v>101</v>
       </c>
-      <c r="D25" s="19" t="s">
+      <c r="E25" s="19" t="s">
         <v>67</v>
       </c>
-      <c r="E25" s="19" t="s">
+      <c r="F25" s="19" t="s">
         <v>42</v>
       </c>
-      <c r="F25" s="20">
+      <c r="G25" s="20">
         <v>2</v>
       </c>
-      <c r="G25" s="17" t="s">
+      <c r="H25" s="17" t="s">
         <v>104</v>
       </c>
-      <c r="H25" s="17" t="s">
+      <c r="I25" s="17" t="s">
         <v>105</v>
       </c>
-      <c r="I25" s="18" t="s">
+      <c r="J25" s="18" t="s">
         <v>106</v>
       </c>
-      <c r="J25" s="17" t="s">
+      <c r="K25" s="17" t="s">
         <v>107</v>
       </c>
     </row>
-    <row r="26" spans="1:10" ht="33" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:11" ht="33" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A26" s="21" t="str">
-        <f t="shared" si="0"/>
+        <f>H26&amp;G26&amp;I26&amp;C26&amp;"'"&amp;J26&amp;D26&amp;K26</f>
         <v xml:space="preserve"> for (int i = 0; i &lt;1 ; i++) {
             tileSet.add(new Tile('Z', 11));
         }
         </v>
       </c>
-      <c r="B26" s="19" t="s">
+      <c r="B26" s="24" t="str">
+        <f t="shared" si="0"/>
+        <v>tileSetMap.put('Z', 11);</v>
+      </c>
+      <c r="C26" s="19" t="s">
         <v>102</v>
       </c>
-      <c r="C26" s="19" t="s">
+      <c r="D26" s="19" t="s">
         <v>103</v>
       </c>
-      <c r="D26" s="19" t="s">
+      <c r="E26" s="19" t="s">
         <v>68</v>
       </c>
-      <c r="E26" s="19" t="s">
+      <c r="F26" s="19" t="s">
         <v>42</v>
       </c>
-      <c r="F26" s="20">
+      <c r="G26" s="20">
         <v>1</v>
       </c>
-      <c r="G26" s="17" t="s">
+      <c r="H26" s="17" t="s">
         <v>104</v>
       </c>
-      <c r="H26" s="17" t="s">
+      <c r="I26" s="17" t="s">
         <v>105</v>
       </c>
-      <c r="I26" s="18" t="s">
+      <c r="J26" s="18" t="s">
         <v>106</v>
       </c>
-      <c r="J26" s="17" t="s">
+      <c r="K26" s="17" t="s">
         <v>107</v>
       </c>
     </row>
-    <row r="27" spans="1:10" ht="33" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:11" ht="33" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A27" s="21" t="str">
-        <f t="shared" si="0"/>
+        <f>H27&amp;G27&amp;I27&amp;C27&amp;"'"&amp;J27&amp;D27&amp;K27</f>
         <v xml:space="preserve"> for (int i = 0; i &lt;5 ; i++) {
             tileSet.add(new Tile('_', 5));
         }
         </v>
       </c>
-      <c r="B27" s="19" t="s">
+      <c r="B27" s="24" t="str">
+        <f t="shared" si="0"/>
+        <v>tileSetMap.put('_', 5);</v>
+      </c>
+      <c r="C27" s="19" t="s">
         <v>108</v>
       </c>
-      <c r="C27" s="19">
+      <c r="D27" s="19">
         <v>5</v>
       </c>
-      <c r="D27" s="19" t="s">
+      <c r="E27" s="19" t="s">
         <v>109</v>
       </c>
-      <c r="E27" s="19" t="s">
+      <c r="F27" s="19" t="s">
         <v>42</v>
       </c>
-      <c r="F27" s="19">
+      <c r="G27" s="19">
         <v>5</v>
       </c>
-      <c r="G27" s="17" t="s">
+      <c r="H27" s="17" t="s">
         <v>104</v>
       </c>
-      <c r="H27" s="17" t="s">
+      <c r="I27" s="17" t="s">
         <v>105</v>
       </c>
-      <c r="I27" s="18" t="s">
+      <c r="J27" s="18" t="s">
         <v>106</v>
       </c>
-      <c r="J27" s="17" t="s">
+      <c r="K27" s="17" t="s">
         <v>107</v>
       </c>
     </row>

</xml_diff>